<commit_message>
Fixed the mac compatibility problem with xlwings
</commit_message>
<xml_diff>
--- a/Opportunities/Pipeline_monitor/Pipeline_monitor.xlsx
+++ b/Opportunities/Pipeline_monitor/Pipeline_monitor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jerry.chen\PycharmProjects\pythonProject\Opportunities\Pipeline_monitor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kamanl/PycharmProjects/Investing_project/Opportunities/Pipeline_monitor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0088E6-06CC-4762-ACFA-A9FA88E61ED6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{427ADB3E-6524-A94C-AE93-FB0ADCB7A7EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Monitor" sheetId="1" r:id="rId1"/>
@@ -20,14 +20,17 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Current_Holdings!$B$6:$J$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Monitor!$B$4:$N$4</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
   <si>
     <t>Pipeline Monitor</t>
   </si>
@@ -71,21 +74,6 @@
   </si>
   <si>
     <t>Status</t>
-  </si>
-  <si>
-    <t>0806.HK</t>
-  </si>
-  <si>
-    <t>VALUE PARTNERS</t>
-  </si>
-  <si>
-    <t>HKG</t>
-  </si>
-  <si>
-    <t>6186.HK</t>
-  </si>
-  <si>
-    <t>CHINA FEIHE</t>
   </si>
   <si>
     <t>Current Holdings Monitor</t>
@@ -127,16 +115,40 @@
     <t xml:space="preserve">Total Protfolio at FV = </t>
   </si>
   <si>
+    <t>0806.HK</t>
+  </si>
+  <si>
+    <t>VALUE PARTNERS</t>
+  </si>
+  <si>
+    <t>HKG</t>
+  </si>
+  <si>
     <t>1475.HK</t>
   </si>
   <si>
     <t>NISSIN FOODS</t>
   </si>
   <si>
-    <t>1766.HK</t>
+    <t>603338.SS</t>
   </si>
   <si>
-    <t>CRRC</t>
+    <t>ZHEJIANG DINGLI MACHINERY CO LT</t>
+  </si>
+  <si>
+    <t>SHH</t>
+  </si>
+  <si>
+    <t>3718.HK</t>
+  </si>
+  <si>
+    <t>BJ ENT URBAN</t>
+  </si>
+  <si>
+    <t>0697.HK</t>
+  </si>
+  <si>
+    <t>SHOUCHENG</t>
   </si>
 </sst>
 </file>
@@ -166,6 +178,7 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -671,20 +684,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:N200"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.453125" customWidth="1"/>
-    <col min="2" max="11" width="14.6328125" customWidth="1"/>
-    <col min="12" max="12" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.7265625" customWidth="1"/>
-    <col min="14" max="14" width="14.6328125" customWidth="1"/>
+    <col min="1" max="1" width="2.5" customWidth="1"/>
+    <col min="2" max="11" width="14.6640625" customWidth="1"/>
+    <col min="12" max="12" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.6640625" customWidth="1"/>
+    <col min="14" max="14" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -702,7 +715,7 @@
       <c r="M2" s="15"/>
       <c r="N2" s="15"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
@@ -725,7 +738,7 @@
         <v>7</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>8</v>
@@ -737,41 +750,41 @@
         <v>10</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B5" s="5" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="E5" s="7">
-        <v>2.6</v>
+        <v>0.66</v>
       </c>
       <c r="F5" s="6">
-        <v>0.3072047302954104</v>
+        <v>1.0970527454262955</v>
       </c>
       <c r="G5" s="6">
-        <v>0.13489889552202361</v>
+        <v>0.19492479482945849</v>
       </c>
       <c r="H5" s="6">
         <f>F5-G5</f>
-        <v>0.17230583477338679</v>
+        <v>0.90212795059683704</v>
       </c>
       <c r="I5" s="5">
         <v>0.14560000000000001</v>
       </c>
       <c r="J5" s="6">
         <f>I5/E5</f>
-        <v>5.6000000000000001E-2</v>
+        <v>0.22060606060606061</v>
       </c>
       <c r="K5" s="7">
         <v>5.3</v>
@@ -779,137 +792,171 @@
       <c r="L5" s="8">
         <v>44925</v>
       </c>
-      <c r="M5" s="8"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="M5" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="E6" s="7">
-        <v>6.54</v>
+        <v>2.6</v>
       </c>
       <c r="F6" s="6">
-        <v>4.981606450514553E-2</v>
+        <v>5.7459512467880058E-2</v>
       </c>
       <c r="G6" s="6">
-        <v>0.10891423458942941</v>
+        <v>9.3811838619443283E-2</v>
       </c>
       <c r="H6" s="6">
         <f>F6-G6</f>
-        <v>-5.9098170084283877E-2</v>
+        <v>-3.6352326151563225E-2</v>
       </c>
       <c r="I6" s="5">
-        <v>0.14560000000000001</v>
+        <v>0</v>
       </c>
       <c r="J6" s="6">
         <f>I6/E6</f>
-        <v>2.2262996941896027E-2</v>
+        <v>0</v>
       </c>
       <c r="K6" s="7">
-        <v>5.3</v>
+        <v>2.12</v>
       </c>
       <c r="L6" s="8">
-        <v>45015</v>
-      </c>
-      <c r="M6" s="8"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+        <v>44925</v>
+      </c>
+      <c r="M6" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B7" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="E7" s="7">
-        <v>3.11</v>
+        <v>6.54</v>
       </c>
       <c r="F7" s="6">
-        <v>-0.32818777766352203</v>
+        <v>4.9815184991756523E-2</v>
       </c>
       <c r="G7" s="6">
-        <v>0.27236067307556133</v>
+        <v>9.7090573713234762E-2</v>
       </c>
       <c r="H7" s="6">
         <f>F7-G7</f>
-        <v>-0.60054845073908336</v>
+        <v>-4.727538872147824E-2</v>
       </c>
       <c r="I7" s="5">
         <v>0.14560000000000001</v>
       </c>
       <c r="J7" s="6">
         <f>I7/E7</f>
-        <v>4.6816720257234733E-2</v>
+        <v>2.2262996941896027E-2</v>
       </c>
       <c r="K7" s="7">
-        <v>5.3</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="L7" s="8">
         <v>45015</v>
       </c>
-      <c r="M7" s="8"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="M7" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B8" s="5" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="E8" s="7">
-        <v>6.61</v>
+        <v>53.88</v>
       </c>
       <c r="F8" s="6">
-        <v>-0.68464668619756364</v>
+        <v>-0.28739529366053429</v>
       </c>
       <c r="G8" s="6">
-        <v>7.1411065827984785</v>
+        <v>8.167411802127264E-2</v>
       </c>
       <c r="H8" s="6">
         <f>F8-G8</f>
-        <v>-7.8257532689960421</v>
+        <v>-0.36906941168180696</v>
       </c>
       <c r="I8" s="5">
         <v>0.14560000000000001</v>
       </c>
       <c r="J8" s="6">
         <f>I8/E8</f>
-        <v>2.2027231467473526E-2</v>
+        <v>2.7023014105419449E-3</v>
       </c>
       <c r="K8" s="7">
         <v>5.3</v>
       </c>
       <c r="L8" s="8">
+        <v>45015</v>
+      </c>
+      <c r="M8" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="7">
+        <v>1.74</v>
+      </c>
+      <c r="F9" s="6">
+        <v>-0.25796975571396996</v>
+      </c>
+      <c r="G9" s="6">
+        <v>0.35888736715901126</v>
+      </c>
+      <c r="H9" s="6">
+        <f>F9-G9</f>
+        <v>-0.61685712287298122</v>
+      </c>
+      <c r="I9" s="5">
+        <v>0.14560000000000001</v>
+      </c>
+      <c r="J9" s="6">
+        <f>I9/E9</f>
+        <v>8.3678160919540237E-2</v>
+      </c>
+      <c r="K9" s="7">
+        <v>5.3</v>
+      </c>
+      <c r="L9" s="8">
         <v>44925</v>
       </c>
-      <c r="M8" s="8"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="M9" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -923,7 +970,7 @@
       <c r="L10" s="8"/>
       <c r="M10" s="8"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -937,7 +984,7 @@
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -951,7 +998,7 @@
       <c r="L12" s="8"/>
       <c r="M12" s="8"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -965,7 +1012,7 @@
       <c r="L13" s="8"/>
       <c r="M13" s="8"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -979,7 +1026,7 @@
       <c r="L14" s="8"/>
       <c r="M14" s="8"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -993,7 +1040,7 @@
       <c r="L15" s="8"/>
       <c r="M15" s="8"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -1007,7 +1054,7 @@
       <c r="L16" s="8"/>
       <c r="M16" s="8"/>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -1021,7 +1068,7 @@
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -1035,7 +1082,7 @@
       <c r="L18" s="8"/>
       <c r="M18" s="8"/>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -1049,7 +1096,7 @@
       <c r="L19" s="8"/>
       <c r="M19" s="8"/>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
@@ -1063,7 +1110,7 @@
       <c r="L20" s="8"/>
       <c r="M20" s="8"/>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
@@ -1077,7 +1124,7 @@
       <c r="L21" s="8"/>
       <c r="M21" s="8"/>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
@@ -1091,7 +1138,7 @@
       <c r="L22" s="8"/>
       <c r="M22" s="8"/>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -1105,7 +1152,7 @@
       <c r="L23" s="8"/>
       <c r="M23" s="8"/>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -1119,7 +1166,7 @@
       <c r="L24" s="8"/>
       <c r="M24" s="8"/>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
@@ -1133,7 +1180,7 @@
       <c r="L25" s="8"/>
       <c r="M25" s="8"/>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
@@ -1147,7 +1194,7 @@
       <c r="L26" s="8"/>
       <c r="M26" s="8"/>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
@@ -1161,7 +1208,7 @@
       <c r="L27" s="8"/>
       <c r="M27" s="8"/>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
@@ -1175,7 +1222,7 @@
       <c r="L28" s="8"/>
       <c r="M28" s="8"/>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
@@ -1189,7 +1236,7 @@
       <c r="L29" s="8"/>
       <c r="M29" s="8"/>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
@@ -1203,7 +1250,7 @@
       <c r="L30" s="8"/>
       <c r="M30" s="8"/>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
@@ -1217,7 +1264,7 @@
       <c r="L31" s="8"/>
       <c r="M31" s="8"/>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -1231,7 +1278,7 @@
       <c r="L32" s="8"/>
       <c r="M32" s="8"/>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
@@ -1245,7 +1292,7 @@
       <c r="L33" s="8"/>
       <c r="M33" s="8"/>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -1259,7 +1306,7 @@
       <c r="L34" s="8"/>
       <c r="M34" s="8"/>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
@@ -1273,7 +1320,7 @@
       <c r="L35" s="8"/>
       <c r="M35" s="8"/>
     </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
@@ -1287,7 +1334,7 @@
       <c r="L36" s="8"/>
       <c r="M36" s="8"/>
     </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
@@ -1301,7 +1348,7 @@
       <c r="L37" s="8"/>
       <c r="M37" s="8"/>
     </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
@@ -1315,7 +1362,7 @@
       <c r="L38" s="8"/>
       <c r="M38" s="8"/>
     </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
@@ -1329,7 +1376,7 @@
       <c r="L39" s="8"/>
       <c r="M39" s="8"/>
     </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
@@ -1343,7 +1390,7 @@
       <c r="L40" s="8"/>
       <c r="M40" s="8"/>
     </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
@@ -1357,7 +1404,7 @@
       <c r="L41" s="8"/>
       <c r="M41" s="8"/>
     </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
@@ -1371,7 +1418,7 @@
       <c r="L42" s="8"/>
       <c r="M42" s="8"/>
     </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
@@ -1385,7 +1432,7 @@
       <c r="L43" s="8"/>
       <c r="M43" s="8"/>
     </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
@@ -1399,7 +1446,7 @@
       <c r="L44" s="8"/>
       <c r="M44" s="8"/>
     </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
@@ -1413,7 +1460,7 @@
       <c r="L45" s="8"/>
       <c r="M45" s="8"/>
     </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
@@ -1427,7 +1474,7 @@
       <c r="L46" s="8"/>
       <c r="M46" s="8"/>
     </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
@@ -1441,7 +1488,7 @@
       <c r="L47" s="8"/>
       <c r="M47" s="8"/>
     </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
@@ -1455,7 +1502,7 @@
       <c r="L48" s="8"/>
       <c r="M48" s="8"/>
     </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
@@ -1469,7 +1516,7 @@
       <c r="L49" s="8"/>
       <c r="M49" s="8"/>
     </row>
-    <row r="50" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
@@ -1483,7 +1530,7 @@
       <c r="L50" s="8"/>
       <c r="M50" s="8"/>
     </row>
-    <row r="51" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
@@ -1497,7 +1544,7 @@
       <c r="L51" s="8"/>
       <c r="M51" s="8"/>
     </row>
-    <row r="52" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
@@ -1511,7 +1558,7 @@
       <c r="L52" s="8"/>
       <c r="M52" s="8"/>
     </row>
-    <row r="53" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
@@ -1525,7 +1572,7 @@
       <c r="L53" s="8"/>
       <c r="M53" s="8"/>
     </row>
-    <row r="54" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
@@ -1539,7 +1586,7 @@
       <c r="L54" s="8"/>
       <c r="M54" s="8"/>
     </row>
-    <row r="55" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
@@ -1553,7 +1600,7 @@
       <c r="L55" s="8"/>
       <c r="M55" s="8"/>
     </row>
-    <row r="56" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
@@ -1567,7 +1614,7 @@
       <c r="L56" s="8"/>
       <c r="M56" s="8"/>
     </row>
-    <row r="57" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
@@ -1581,7 +1628,7 @@
       <c r="L57" s="8"/>
       <c r="M57" s="8"/>
     </row>
-    <row r="58" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
@@ -1595,7 +1642,7 @@
       <c r="L58" s="8"/>
       <c r="M58" s="8"/>
     </row>
-    <row r="59" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
       <c r="D59" s="5"/>
@@ -1609,7 +1656,7 @@
       <c r="L59" s="8"/>
       <c r="M59" s="8"/>
     </row>
-    <row r="60" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
@@ -1623,7 +1670,7 @@
       <c r="L60" s="8"/>
       <c r="M60" s="8"/>
     </row>
-    <row r="61" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
@@ -1637,7 +1684,7 @@
       <c r="L61" s="8"/>
       <c r="M61" s="8"/>
     </row>
-    <row r="62" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
@@ -1651,7 +1698,7 @@
       <c r="L62" s="8"/>
       <c r="M62" s="8"/>
     </row>
-    <row r="63" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
@@ -1665,7 +1712,7 @@
       <c r="L63" s="8"/>
       <c r="M63" s="8"/>
     </row>
-    <row r="64" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
@@ -1679,7 +1726,7 @@
       <c r="L64" s="8"/>
       <c r="M64" s="8"/>
     </row>
-    <row r="65" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B65" s="5"/>
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
@@ -1693,7 +1740,7 @@
       <c r="L65" s="8"/>
       <c r="M65" s="8"/>
     </row>
-    <row r="66" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
@@ -1707,7 +1754,7 @@
       <c r="L66" s="8"/>
       <c r="M66" s="8"/>
     </row>
-    <row r="67" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
       <c r="D67" s="5"/>
@@ -1721,7 +1768,7 @@
       <c r="L67" s="8"/>
       <c r="M67" s="8"/>
     </row>
-    <row r="68" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
@@ -1735,7 +1782,7 @@
       <c r="L68" s="8"/>
       <c r="M68" s="8"/>
     </row>
-    <row r="69" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B69" s="5"/>
       <c r="C69" s="5"/>
       <c r="D69" s="5"/>
@@ -1749,7 +1796,7 @@
       <c r="L69" s="8"/>
       <c r="M69" s="8"/>
     </row>
-    <row r="70" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B70" s="5"/>
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
@@ -1763,7 +1810,7 @@
       <c r="L70" s="8"/>
       <c r="M70" s="8"/>
     </row>
-    <row r="71" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B71" s="5"/>
       <c r="C71" s="5"/>
       <c r="D71" s="5"/>
@@ -1777,7 +1824,7 @@
       <c r="L71" s="8"/>
       <c r="M71" s="8"/>
     </row>
-    <row r="72" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
@@ -1791,7 +1838,7 @@
       <c r="L72" s="8"/>
       <c r="M72" s="8"/>
     </row>
-    <row r="73" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B73" s="5"/>
       <c r="C73" s="5"/>
       <c r="D73" s="5"/>
@@ -1805,7 +1852,7 @@
       <c r="L73" s="8"/>
       <c r="M73" s="8"/>
     </row>
-    <row r="74" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B74" s="5"/>
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
@@ -1819,7 +1866,7 @@
       <c r="L74" s="8"/>
       <c r="M74" s="8"/>
     </row>
-    <row r="75" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B75" s="5"/>
       <c r="C75" s="5"/>
       <c r="D75" s="5"/>
@@ -1833,7 +1880,7 @@
       <c r="L75" s="8"/>
       <c r="M75" s="8"/>
     </row>
-    <row r="76" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B76" s="5"/>
       <c r="C76" s="5"/>
       <c r="D76" s="5"/>
@@ -1847,7 +1894,7 @@
       <c r="L76" s="8"/>
       <c r="M76" s="8"/>
     </row>
-    <row r="77" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B77" s="5"/>
       <c r="C77" s="5"/>
       <c r="D77" s="5"/>
@@ -1861,7 +1908,7 @@
       <c r="L77" s="8"/>
       <c r="M77" s="8"/>
     </row>
-    <row r="78" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B78" s="5"/>
       <c r="C78" s="5"/>
       <c r="D78" s="5"/>
@@ -1875,7 +1922,7 @@
       <c r="L78" s="8"/>
       <c r="M78" s="8"/>
     </row>
-    <row r="79" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B79" s="5"/>
       <c r="C79" s="5"/>
       <c r="D79" s="5"/>
@@ -1889,7 +1936,7 @@
       <c r="L79" s="8"/>
       <c r="M79" s="8"/>
     </row>
-    <row r="80" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B80" s="5"/>
       <c r="C80" s="5"/>
       <c r="D80" s="5"/>
@@ -1903,7 +1950,7 @@
       <c r="L80" s="8"/>
       <c r="M80" s="8"/>
     </row>
-    <row r="81" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B81" s="5"/>
       <c r="C81" s="5"/>
       <c r="D81" s="5"/>
@@ -1917,7 +1964,7 @@
       <c r="L81" s="8"/>
       <c r="M81" s="8"/>
     </row>
-    <row r="82" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B82" s="5"/>
       <c r="C82" s="5"/>
       <c r="D82" s="5"/>
@@ -1931,7 +1978,7 @@
       <c r="L82" s="8"/>
       <c r="M82" s="8"/>
     </row>
-    <row r="83" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B83" s="5"/>
       <c r="C83" s="5"/>
       <c r="D83" s="5"/>
@@ -1945,7 +1992,7 @@
       <c r="L83" s="8"/>
       <c r="M83" s="8"/>
     </row>
-    <row r="84" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B84" s="5"/>
       <c r="C84" s="5"/>
       <c r="D84" s="5"/>
@@ -1959,7 +2006,7 @@
       <c r="L84" s="8"/>
       <c r="M84" s="8"/>
     </row>
-    <row r="85" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B85" s="5"/>
       <c r="C85" s="5"/>
       <c r="D85" s="5"/>
@@ -1973,7 +2020,7 @@
       <c r="L85" s="8"/>
       <c r="M85" s="8"/>
     </row>
-    <row r="86" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
       <c r="D86" s="5"/>
@@ -1987,7 +2034,7 @@
       <c r="L86" s="8"/>
       <c r="M86" s="8"/>
     </row>
-    <row r="87" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B87" s="5"/>
       <c r="C87" s="5"/>
       <c r="D87" s="5"/>
@@ -2001,7 +2048,7 @@
       <c r="L87" s="8"/>
       <c r="M87" s="8"/>
     </row>
-    <row r="88" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B88" s="5"/>
       <c r="C88" s="5"/>
       <c r="D88" s="5"/>
@@ -2015,7 +2062,7 @@
       <c r="L88" s="8"/>
       <c r="M88" s="8"/>
     </row>
-    <row r="89" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B89" s="5"/>
       <c r="C89" s="5"/>
       <c r="D89" s="5"/>
@@ -2029,7 +2076,7 @@
       <c r="L89" s="8"/>
       <c r="M89" s="8"/>
     </row>
-    <row r="90" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B90" s="5"/>
       <c r="C90" s="5"/>
       <c r="D90" s="5"/>
@@ -2043,7 +2090,7 @@
       <c r="L90" s="8"/>
       <c r="M90" s="8"/>
     </row>
-    <row r="91" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B91" s="5"/>
       <c r="C91" s="5"/>
       <c r="D91" s="5"/>
@@ -2057,7 +2104,7 @@
       <c r="L91" s="8"/>
       <c r="M91" s="8"/>
     </row>
-    <row r="92" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B92" s="5"/>
       <c r="C92" s="5"/>
       <c r="D92" s="5"/>
@@ -2071,7 +2118,7 @@
       <c r="L92" s="8"/>
       <c r="M92" s="8"/>
     </row>
-    <row r="93" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B93" s="5"/>
       <c r="C93" s="5"/>
       <c r="D93" s="5"/>
@@ -2085,7 +2132,7 @@
       <c r="L93" s="8"/>
       <c r="M93" s="8"/>
     </row>
-    <row r="94" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B94" s="5"/>
       <c r="C94" s="5"/>
       <c r="D94" s="5"/>
@@ -2099,7 +2146,7 @@
       <c r="L94" s="8"/>
       <c r="M94" s="8"/>
     </row>
-    <row r="95" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B95" s="5"/>
       <c r="C95" s="5"/>
       <c r="D95" s="5"/>
@@ -2113,7 +2160,7 @@
       <c r="L95" s="8"/>
       <c r="M95" s="8"/>
     </row>
-    <row r="96" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B96" s="5"/>
       <c r="C96" s="5"/>
       <c r="D96" s="5"/>
@@ -2127,7 +2174,7 @@
       <c r="L96" s="8"/>
       <c r="M96" s="8"/>
     </row>
-    <row r="97" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B97" s="5"/>
       <c r="C97" s="5"/>
       <c r="D97" s="5"/>
@@ -2141,7 +2188,7 @@
       <c r="L97" s="8"/>
       <c r="M97" s="8"/>
     </row>
-    <row r="98" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B98" s="5"/>
       <c r="C98" s="5"/>
       <c r="D98" s="5"/>
@@ -2155,7 +2202,7 @@
       <c r="L98" s="8"/>
       <c r="M98" s="8"/>
     </row>
-    <row r="99" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="99" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B99" s="5"/>
       <c r="C99" s="5"/>
       <c r="D99" s="5"/>
@@ -2169,7 +2216,7 @@
       <c r="L99" s="8"/>
       <c r="M99" s="8"/>
     </row>
-    <row r="100" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B100" s="5"/>
       <c r="C100" s="5"/>
       <c r="D100" s="5"/>
@@ -2183,7 +2230,7 @@
       <c r="L100" s="8"/>
       <c r="M100" s="8"/>
     </row>
-    <row r="101" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B101" s="5"/>
       <c r="C101" s="5"/>
       <c r="D101" s="5"/>
@@ -2197,7 +2244,7 @@
       <c r="L101" s="8"/>
       <c r="M101" s="8"/>
     </row>
-    <row r="102" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B102" s="5"/>
       <c r="C102" s="5"/>
       <c r="D102" s="5"/>
@@ -2211,7 +2258,7 @@
       <c r="L102" s="8"/>
       <c r="M102" s="8"/>
     </row>
-    <row r="103" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="103" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B103" s="5"/>
       <c r="C103" s="5"/>
       <c r="D103" s="5"/>
@@ -2225,7 +2272,7 @@
       <c r="L103" s="8"/>
       <c r="M103" s="8"/>
     </row>
-    <row r="104" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B104" s="5"/>
       <c r="C104" s="5"/>
       <c r="D104" s="5"/>
@@ -2239,7 +2286,7 @@
       <c r="L104" s="8"/>
       <c r="M104" s="8"/>
     </row>
-    <row r="105" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B105" s="5"/>
       <c r="C105" s="5"/>
       <c r="D105" s="5"/>
@@ -2253,7 +2300,7 @@
       <c r="L105" s="8"/>
       <c r="M105" s="8"/>
     </row>
-    <row r="106" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B106" s="5"/>
       <c r="C106" s="5"/>
       <c r="D106" s="5"/>
@@ -2267,7 +2314,7 @@
       <c r="L106" s="8"/>
       <c r="M106" s="8"/>
     </row>
-    <row r="107" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B107" s="5"/>
       <c r="C107" s="5"/>
       <c r="D107" s="5"/>
@@ -2281,7 +2328,7 @@
       <c r="L107" s="8"/>
       <c r="M107" s="8"/>
     </row>
-    <row r="108" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B108" s="5"/>
       <c r="C108" s="5"/>
       <c r="D108" s="5"/>
@@ -2295,7 +2342,7 @@
       <c r="L108" s="8"/>
       <c r="M108" s="8"/>
     </row>
-    <row r="109" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B109" s="5"/>
       <c r="C109" s="5"/>
       <c r="D109" s="5"/>
@@ -2309,7 +2356,7 @@
       <c r="L109" s="8"/>
       <c r="M109" s="8"/>
     </row>
-    <row r="110" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="110" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B110" s="5"/>
       <c r="C110" s="5"/>
       <c r="D110" s="5"/>
@@ -2323,7 +2370,7 @@
       <c r="L110" s="8"/>
       <c r="M110" s="8"/>
     </row>
-    <row r="111" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="111" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B111" s="5"/>
       <c r="C111" s="5"/>
       <c r="D111" s="5"/>
@@ -2337,7 +2384,7 @@
       <c r="L111" s="8"/>
       <c r="M111" s="8"/>
     </row>
-    <row r="112" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="112" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B112" s="5"/>
       <c r="C112" s="5"/>
       <c r="D112" s="5"/>
@@ -2351,7 +2398,7 @@
       <c r="L112" s="8"/>
       <c r="M112" s="8"/>
     </row>
-    <row r="113" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="113" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B113" s="5"/>
       <c r="C113" s="5"/>
       <c r="D113" s="5"/>
@@ -2365,7 +2412,7 @@
       <c r="L113" s="8"/>
       <c r="M113" s="8"/>
     </row>
-    <row r="114" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="114" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B114" s="5"/>
       <c r="C114" s="5"/>
       <c r="D114" s="5"/>
@@ -2379,7 +2426,7 @@
       <c r="L114" s="8"/>
       <c r="M114" s="8"/>
     </row>
-    <row r="115" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="115" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B115" s="5"/>
       <c r="C115" s="5"/>
       <c r="D115" s="5"/>
@@ -2393,7 +2440,7 @@
       <c r="L115" s="8"/>
       <c r="M115" s="8"/>
     </row>
-    <row r="116" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="116" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B116" s="5"/>
       <c r="C116" s="5"/>
       <c r="D116" s="5"/>
@@ -2407,7 +2454,7 @@
       <c r="L116" s="8"/>
       <c r="M116" s="8"/>
     </row>
-    <row r="117" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="117" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B117" s="5"/>
       <c r="C117" s="5"/>
       <c r="D117" s="5"/>
@@ -2421,7 +2468,7 @@
       <c r="L117" s="8"/>
       <c r="M117" s="8"/>
     </row>
-    <row r="118" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="118" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B118" s="5"/>
       <c r="C118" s="5"/>
       <c r="D118" s="5"/>
@@ -2435,7 +2482,7 @@
       <c r="L118" s="8"/>
       <c r="M118" s="8"/>
     </row>
-    <row r="119" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="119" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B119" s="5"/>
       <c r="C119" s="5"/>
       <c r="D119" s="5"/>
@@ -2449,7 +2496,7 @@
       <c r="L119" s="8"/>
       <c r="M119" s="8"/>
     </row>
-    <row r="120" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="120" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B120" s="5"/>
       <c r="C120" s="5"/>
       <c r="D120" s="5"/>
@@ -2463,7 +2510,7 @@
       <c r="L120" s="8"/>
       <c r="M120" s="8"/>
     </row>
-    <row r="121" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="121" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B121" s="5"/>
       <c r="C121" s="5"/>
       <c r="D121" s="5"/>
@@ -2477,7 +2524,7 @@
       <c r="L121" s="8"/>
       <c r="M121" s="8"/>
     </row>
-    <row r="122" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="122" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B122" s="5"/>
       <c r="C122" s="5"/>
       <c r="D122" s="5"/>
@@ -2491,7 +2538,7 @@
       <c r="L122" s="8"/>
       <c r="M122" s="8"/>
     </row>
-    <row r="123" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="123" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B123" s="5"/>
       <c r="C123" s="5"/>
       <c r="D123" s="5"/>
@@ -2505,7 +2552,7 @@
       <c r="L123" s="8"/>
       <c r="M123" s="8"/>
     </row>
-    <row r="124" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="124" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B124" s="5"/>
       <c r="C124" s="5"/>
       <c r="D124" s="5"/>
@@ -2519,7 +2566,7 @@
       <c r="L124" s="8"/>
       <c r="M124" s="8"/>
     </row>
-    <row r="125" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="125" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B125" s="5"/>
       <c r="C125" s="5"/>
       <c r="D125" s="5"/>
@@ -2533,7 +2580,7 @@
       <c r="L125" s="8"/>
       <c r="M125" s="8"/>
     </row>
-    <row r="126" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="126" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B126" s="5"/>
       <c r="C126" s="5"/>
       <c r="D126" s="5"/>
@@ -2547,7 +2594,7 @@
       <c r="L126" s="8"/>
       <c r="M126" s="8"/>
     </row>
-    <row r="127" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="127" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B127" s="5"/>
       <c r="C127" s="5"/>
       <c r="D127" s="5"/>
@@ -2561,7 +2608,7 @@
       <c r="L127" s="8"/>
       <c r="M127" s="8"/>
     </row>
-    <row r="128" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="128" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B128" s="5"/>
       <c r="C128" s="5"/>
       <c r="D128" s="5"/>
@@ -2575,7 +2622,7 @@
       <c r="L128" s="8"/>
       <c r="M128" s="8"/>
     </row>
-    <row r="129" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="129" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B129" s="5"/>
       <c r="C129" s="5"/>
       <c r="D129" s="5"/>
@@ -2589,7 +2636,7 @@
       <c r="L129" s="8"/>
       <c r="M129" s="8"/>
     </row>
-    <row r="130" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="130" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B130" s="5"/>
       <c r="C130" s="5"/>
       <c r="D130" s="5"/>
@@ -2603,7 +2650,7 @@
       <c r="L130" s="8"/>
       <c r="M130" s="8"/>
     </row>
-    <row r="131" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="131" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B131" s="5"/>
       <c r="C131" s="5"/>
       <c r="D131" s="5"/>
@@ -2617,7 +2664,7 @@
       <c r="L131" s="8"/>
       <c r="M131" s="8"/>
     </row>
-    <row r="132" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="132" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B132" s="5"/>
       <c r="C132" s="5"/>
       <c r="D132" s="5"/>
@@ -2631,7 +2678,7 @@
       <c r="L132" s="8"/>
       <c r="M132" s="8"/>
     </row>
-    <row r="133" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="133" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B133" s="5"/>
       <c r="C133" s="5"/>
       <c r="D133" s="5"/>
@@ -2645,7 +2692,7 @@
       <c r="L133" s="8"/>
       <c r="M133" s="8"/>
     </row>
-    <row r="134" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="134" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B134" s="5"/>
       <c r="C134" s="5"/>
       <c r="D134" s="5"/>
@@ -2659,7 +2706,7 @@
       <c r="L134" s="8"/>
       <c r="M134" s="8"/>
     </row>
-    <row r="135" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="135" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B135" s="5"/>
       <c r="C135" s="5"/>
       <c r="D135" s="5"/>
@@ -2673,7 +2720,7 @@
       <c r="L135" s="8"/>
       <c r="M135" s="8"/>
     </row>
-    <row r="136" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="136" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B136" s="5"/>
       <c r="C136" s="5"/>
       <c r="D136" s="5"/>
@@ -2687,7 +2734,7 @@
       <c r="L136" s="8"/>
       <c r="M136" s="8"/>
     </row>
-    <row r="137" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="137" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B137" s="5"/>
       <c r="C137" s="5"/>
       <c r="D137" s="5"/>
@@ -2701,7 +2748,7 @@
       <c r="L137" s="8"/>
       <c r="M137" s="8"/>
     </row>
-    <row r="138" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="138" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B138" s="5"/>
       <c r="C138" s="5"/>
       <c r="D138" s="5"/>
@@ -2715,7 +2762,7 @@
       <c r="L138" s="8"/>
       <c r="M138" s="8"/>
     </row>
-    <row r="139" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="139" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B139" s="5"/>
       <c r="C139" s="5"/>
       <c r="D139" s="5"/>
@@ -2729,7 +2776,7 @@
       <c r="L139" s="8"/>
       <c r="M139" s="8"/>
     </row>
-    <row r="140" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="140" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B140" s="5"/>
       <c r="C140" s="5"/>
       <c r="D140" s="5"/>
@@ -2743,7 +2790,7 @@
       <c r="L140" s="8"/>
       <c r="M140" s="8"/>
     </row>
-    <row r="141" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="141" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B141" s="5"/>
       <c r="C141" s="5"/>
       <c r="D141" s="5"/>
@@ -2757,7 +2804,7 @@
       <c r="L141" s="8"/>
       <c r="M141" s="8"/>
     </row>
-    <row r="142" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="142" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B142" s="5"/>
       <c r="C142" s="5"/>
       <c r="D142" s="5"/>
@@ -2771,7 +2818,7 @@
       <c r="L142" s="8"/>
       <c r="M142" s="8"/>
     </row>
-    <row r="143" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="143" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B143" s="5"/>
       <c r="C143" s="5"/>
       <c r="D143" s="5"/>
@@ -2785,7 +2832,7 @@
       <c r="L143" s="8"/>
       <c r="M143" s="8"/>
     </row>
-    <row r="144" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="144" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B144" s="5"/>
       <c r="C144" s="5"/>
       <c r="D144" s="5"/>
@@ -2799,7 +2846,7 @@
       <c r="L144" s="8"/>
       <c r="M144" s="8"/>
     </row>
-    <row r="145" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="145" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B145" s="5"/>
       <c r="C145" s="5"/>
       <c r="D145" s="5"/>
@@ -2813,7 +2860,7 @@
       <c r="L145" s="8"/>
       <c r="M145" s="8"/>
     </row>
-    <row r="146" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="146" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B146" s="5"/>
       <c r="C146" s="5"/>
       <c r="D146" s="5"/>
@@ -2827,7 +2874,7 @@
       <c r="L146" s="8"/>
       <c r="M146" s="8"/>
     </row>
-    <row r="147" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="147" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B147" s="5"/>
       <c r="C147" s="5"/>
       <c r="D147" s="5"/>
@@ -2841,7 +2888,7 @@
       <c r="L147" s="8"/>
       <c r="M147" s="8"/>
     </row>
-    <row r="148" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="148" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B148" s="5"/>
       <c r="C148" s="5"/>
       <c r="D148" s="5"/>
@@ -2855,7 +2902,7 @@
       <c r="L148" s="8"/>
       <c r="M148" s="8"/>
     </row>
-    <row r="149" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="149" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B149" s="5"/>
       <c r="C149" s="5"/>
       <c r="D149" s="5"/>
@@ -2869,7 +2916,7 @@
       <c r="L149" s="8"/>
       <c r="M149" s="8"/>
     </row>
-    <row r="150" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="150" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B150" s="5"/>
       <c r="C150" s="5"/>
       <c r="D150" s="5"/>
@@ -2883,7 +2930,7 @@
       <c r="L150" s="8"/>
       <c r="M150" s="8"/>
     </row>
-    <row r="151" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="151" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B151" s="5"/>
       <c r="C151" s="5"/>
       <c r="D151" s="5"/>
@@ -2897,7 +2944,7 @@
       <c r="L151" s="8"/>
       <c r="M151" s="8"/>
     </row>
-    <row r="152" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="152" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B152" s="5"/>
       <c r="C152" s="5"/>
       <c r="D152" s="5"/>
@@ -2911,7 +2958,7 @@
       <c r="L152" s="8"/>
       <c r="M152" s="8"/>
     </row>
-    <row r="153" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="153" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B153" s="5"/>
       <c r="C153" s="5"/>
       <c r="D153" s="5"/>
@@ -2925,7 +2972,7 @@
       <c r="L153" s="8"/>
       <c r="M153" s="8"/>
     </row>
-    <row r="154" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="154" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B154" s="5"/>
       <c r="C154" s="5"/>
       <c r="D154" s="5"/>
@@ -2939,7 +2986,7 @@
       <c r="L154" s="8"/>
       <c r="M154" s="8"/>
     </row>
-    <row r="155" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="155" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B155" s="5"/>
       <c r="C155" s="5"/>
       <c r="D155" s="5"/>
@@ -2953,7 +3000,7 @@
       <c r="L155" s="8"/>
       <c r="M155" s="8"/>
     </row>
-    <row r="156" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="156" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B156" s="5"/>
       <c r="C156" s="5"/>
       <c r="D156" s="5"/>
@@ -2967,7 +3014,7 @@
       <c r="L156" s="8"/>
       <c r="M156" s="8"/>
     </row>
-    <row r="157" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="157" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B157" s="5"/>
       <c r="C157" s="5"/>
       <c r="D157" s="5"/>
@@ -2981,7 +3028,7 @@
       <c r="L157" s="8"/>
       <c r="M157" s="8"/>
     </row>
-    <row r="158" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="158" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B158" s="5"/>
       <c r="C158" s="5"/>
       <c r="D158" s="5"/>
@@ -2995,7 +3042,7 @@
       <c r="L158" s="8"/>
       <c r="M158" s="8"/>
     </row>
-    <row r="159" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="159" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B159" s="5"/>
       <c r="C159" s="5"/>
       <c r="D159" s="5"/>
@@ -3009,7 +3056,7 @@
       <c r="L159" s="8"/>
       <c r="M159" s="8"/>
     </row>
-    <row r="160" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="160" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B160" s="5"/>
       <c r="C160" s="5"/>
       <c r="D160" s="5"/>
@@ -3023,7 +3070,7 @@
       <c r="L160" s="8"/>
       <c r="M160" s="8"/>
     </row>
-    <row r="161" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="161" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B161" s="5"/>
       <c r="C161" s="5"/>
       <c r="D161" s="5"/>
@@ -3037,7 +3084,7 @@
       <c r="L161" s="8"/>
       <c r="M161" s="8"/>
     </row>
-    <row r="162" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="162" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B162" s="5"/>
       <c r="C162" s="5"/>
       <c r="D162" s="5"/>
@@ -3051,7 +3098,7 @@
       <c r="L162" s="8"/>
       <c r="M162" s="8"/>
     </row>
-    <row r="163" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="163" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B163" s="5"/>
       <c r="C163" s="5"/>
       <c r="D163" s="5"/>
@@ -3065,7 +3112,7 @@
       <c r="L163" s="8"/>
       <c r="M163" s="8"/>
     </row>
-    <row r="164" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="164" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B164" s="5"/>
       <c r="C164" s="5"/>
       <c r="D164" s="5"/>
@@ -3079,7 +3126,7 @@
       <c r="L164" s="8"/>
       <c r="M164" s="8"/>
     </row>
-    <row r="165" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="165" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B165" s="5"/>
       <c r="C165" s="5"/>
       <c r="D165" s="5"/>
@@ -3093,7 +3140,7 @@
       <c r="L165" s="8"/>
       <c r="M165" s="8"/>
     </row>
-    <row r="166" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="166" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B166" s="5"/>
       <c r="C166" s="5"/>
       <c r="D166" s="5"/>
@@ -3107,7 +3154,7 @@
       <c r="L166" s="8"/>
       <c r="M166" s="8"/>
     </row>
-    <row r="167" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="167" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B167" s="5"/>
       <c r="C167" s="5"/>
       <c r="D167" s="5"/>
@@ -3121,7 +3168,7 @@
       <c r="L167" s="8"/>
       <c r="M167" s="8"/>
     </row>
-    <row r="168" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="168" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B168" s="5"/>
       <c r="C168" s="5"/>
       <c r="D168" s="5"/>
@@ -3135,7 +3182,7 @@
       <c r="L168" s="8"/>
       <c r="M168" s="8"/>
     </row>
-    <row r="169" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="169" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B169" s="5"/>
       <c r="C169" s="5"/>
       <c r="D169" s="5"/>
@@ -3149,7 +3196,7 @@
       <c r="L169" s="8"/>
       <c r="M169" s="8"/>
     </row>
-    <row r="170" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="170" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B170" s="5"/>
       <c r="C170" s="5"/>
       <c r="D170" s="5"/>
@@ -3163,7 +3210,7 @@
       <c r="L170" s="8"/>
       <c r="M170" s="8"/>
     </row>
-    <row r="171" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="171" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B171" s="5"/>
       <c r="C171" s="5"/>
       <c r="D171" s="5"/>
@@ -3177,7 +3224,7 @@
       <c r="L171" s="8"/>
       <c r="M171" s="8"/>
     </row>
-    <row r="172" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="172" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B172" s="5"/>
       <c r="C172" s="5"/>
       <c r="D172" s="5"/>
@@ -3191,7 +3238,7 @@
       <c r="L172" s="8"/>
       <c r="M172" s="8"/>
     </row>
-    <row r="173" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="173" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B173" s="5"/>
       <c r="C173" s="5"/>
       <c r="D173" s="5"/>
@@ -3205,7 +3252,7 @@
       <c r="L173" s="8"/>
       <c r="M173" s="8"/>
     </row>
-    <row r="174" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="174" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B174" s="5"/>
       <c r="C174" s="5"/>
       <c r="D174" s="5"/>
@@ -3219,7 +3266,7 @@
       <c r="L174" s="8"/>
       <c r="M174" s="8"/>
     </row>
-    <row r="175" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="175" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B175" s="5"/>
       <c r="C175" s="5"/>
       <c r="D175" s="5"/>
@@ -3233,7 +3280,7 @@
       <c r="L175" s="8"/>
       <c r="M175" s="8"/>
     </row>
-    <row r="176" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="176" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B176" s="5"/>
       <c r="C176" s="5"/>
       <c r="D176" s="5"/>
@@ -3247,7 +3294,7 @@
       <c r="L176" s="8"/>
       <c r="M176" s="8"/>
     </row>
-    <row r="177" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="177" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B177" s="5"/>
       <c r="C177" s="5"/>
       <c r="D177" s="5"/>
@@ -3261,7 +3308,7 @@
       <c r="L177" s="8"/>
       <c r="M177" s="8"/>
     </row>
-    <row r="178" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="178" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B178" s="5"/>
       <c r="C178" s="5"/>
       <c r="D178" s="5"/>
@@ -3275,7 +3322,7 @@
       <c r="L178" s="8"/>
       <c r="M178" s="8"/>
     </row>
-    <row r="179" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="179" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B179" s="5"/>
       <c r="C179" s="5"/>
       <c r="D179" s="5"/>
@@ -3289,7 +3336,7 @@
       <c r="L179" s="8"/>
       <c r="M179" s="8"/>
     </row>
-    <row r="180" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="180" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B180" s="5"/>
       <c r="C180" s="5"/>
       <c r="D180" s="5"/>
@@ -3303,7 +3350,7 @@
       <c r="L180" s="8"/>
       <c r="M180" s="8"/>
     </row>
-    <row r="181" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="181" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B181" s="5"/>
       <c r="C181" s="5"/>
       <c r="D181" s="5"/>
@@ -3317,7 +3364,7 @@
       <c r="L181" s="8"/>
       <c r="M181" s="8"/>
     </row>
-    <row r="182" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="182" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B182" s="5"/>
       <c r="C182" s="5"/>
       <c r="D182" s="5"/>
@@ -3331,7 +3378,7 @@
       <c r="L182" s="8"/>
       <c r="M182" s="8"/>
     </row>
-    <row r="183" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="183" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B183" s="5"/>
       <c r="C183" s="5"/>
       <c r="D183" s="5"/>
@@ -3345,7 +3392,7 @@
       <c r="L183" s="8"/>
       <c r="M183" s="8"/>
     </row>
-    <row r="184" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="184" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B184" s="5"/>
       <c r="C184" s="5"/>
       <c r="D184" s="5"/>
@@ -3359,7 +3406,7 @@
       <c r="L184" s="8"/>
       <c r="M184" s="8"/>
     </row>
-    <row r="185" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="185" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B185" s="5"/>
       <c r="C185" s="5"/>
       <c r="D185" s="5"/>
@@ -3373,7 +3420,7 @@
       <c r="L185" s="8"/>
       <c r="M185" s="8"/>
     </row>
-    <row r="186" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="186" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B186" s="5"/>
       <c r="C186" s="5"/>
       <c r="D186" s="5"/>
@@ -3387,7 +3434,7 @@
       <c r="L186" s="8"/>
       <c r="M186" s="8"/>
     </row>
-    <row r="187" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="187" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B187" s="5"/>
       <c r="C187" s="5"/>
       <c r="D187" s="5"/>
@@ -3401,7 +3448,7 @@
       <c r="L187" s="8"/>
       <c r="M187" s="8"/>
     </row>
-    <row r="188" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="188" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B188" s="5"/>
       <c r="C188" s="5"/>
       <c r="D188" s="5"/>
@@ -3415,7 +3462,7 @@
       <c r="L188" s="8"/>
       <c r="M188" s="8"/>
     </row>
-    <row r="189" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="189" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B189" s="5"/>
       <c r="C189" s="5"/>
       <c r="D189" s="5"/>
@@ -3429,7 +3476,7 @@
       <c r="L189" s="8"/>
       <c r="M189" s="8"/>
     </row>
-    <row r="190" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="190" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B190" s="5"/>
       <c r="C190" s="5"/>
       <c r="D190" s="5"/>
@@ -3443,7 +3490,7 @@
       <c r="L190" s="8"/>
       <c r="M190" s="8"/>
     </row>
-    <row r="191" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="191" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B191" s="5"/>
       <c r="C191" s="5"/>
       <c r="D191" s="5"/>
@@ -3457,7 +3504,7 @@
       <c r="L191" s="8"/>
       <c r="M191" s="8"/>
     </row>
-    <row r="192" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="192" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B192" s="5"/>
       <c r="C192" s="5"/>
       <c r="D192" s="5"/>
@@ -3471,7 +3518,7 @@
       <c r="L192" s="8"/>
       <c r="M192" s="8"/>
     </row>
-    <row r="193" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="193" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B193" s="5"/>
       <c r="C193" s="5"/>
       <c r="D193" s="5"/>
@@ -3485,7 +3532,7 @@
       <c r="L193" s="8"/>
       <c r="M193" s="8"/>
     </row>
-    <row r="194" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="194" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B194" s="5"/>
       <c r="C194" s="5"/>
       <c r="D194" s="5"/>
@@ -3499,7 +3546,7 @@
       <c r="L194" s="8"/>
       <c r="M194" s="8"/>
     </row>
-    <row r="195" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="195" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B195" s="5"/>
       <c r="C195" s="5"/>
       <c r="D195" s="5"/>
@@ -3513,7 +3560,7 @@
       <c r="L195" s="8"/>
       <c r="M195" s="8"/>
     </row>
-    <row r="196" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="196" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B196" s="5"/>
       <c r="C196" s="5"/>
       <c r="D196" s="5"/>
@@ -3527,7 +3574,7 @@
       <c r="L196" s="8"/>
       <c r="M196" s="8"/>
     </row>
-    <row r="197" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="197" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B197" s="5"/>
       <c r="C197" s="5"/>
       <c r="D197" s="5"/>
@@ -3541,7 +3588,7 @@
       <c r="L197" s="8"/>
       <c r="M197" s="8"/>
     </row>
-    <row r="198" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="198" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B198" s="5"/>
       <c r="C198" s="5"/>
       <c r="D198" s="5"/>
@@ -3555,7 +3602,7 @@
       <c r="L198" s="8"/>
       <c r="M198" s="8"/>
     </row>
-    <row r="199" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="199" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B199" s="5"/>
       <c r="C199" s="5"/>
       <c r="D199" s="5"/>
@@ -3569,7 +3616,7 @@
       <c r="L199" s="8"/>
       <c r="M199" s="8"/>
     </row>
-    <row r="200" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="200" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B200" s="5"/>
       <c r="C200" s="5"/>
       <c r="D200" s="5"/>
@@ -3585,8 +3632,8 @@
     </row>
   </sheetData>
   <autoFilter ref="B4:N4" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:N8">
-      <sortCondition descending="1" ref="H4"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:N9">
+      <sortCondition descending="1" ref="H4:H9"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3598,21 +3645,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA8F8C16-C341-4E22-B58A-1C8A959287DB}">
   <dimension ref="A2:J200"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.453125" customWidth="1"/>
-    <col min="2" max="9" width="14.6328125" customWidth="1"/>
-    <col min="10" max="10" width="15.6328125" customWidth="1"/>
+    <col min="1" max="1" width="2.5" customWidth="1"/>
+    <col min="2" max="9" width="14.6640625" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="13" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
@@ -3620,34 +3667,34 @@
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
       <c r="H2" s="16" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I2" s="19">
         <v>44902</v>
       </c>
       <c r="J2" s="19"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B3" s="10" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="18"/>
       <c r="F3" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B4" s="10" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D4" s="20"/>
       <c r="E4" s="21"/>
       <c r="F4" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>1</v>
       </c>
@@ -3658,36 +3705,36 @@
         <v>3</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>23</v>
       </c>
       <c r="F7" s="7">
         <v>2.2999999999999998</v>
@@ -3702,7 +3749,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -3713,7 +3760,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -3724,7 +3771,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -3735,7 +3782,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -3745,7 +3792,7 @@
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -3755,7 +3802,7 @@
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -3765,7 +3812,7 @@
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -3775,7 +3822,7 @@
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -3785,7 +3832,7 @@
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -3795,7 +3842,7 @@
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -3805,7 +3852,7 @@
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -3815,7 +3862,7 @@
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -3825,7 +3872,7 @@
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
@@ -3835,7 +3882,7 @@
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
@@ -3845,7 +3892,7 @@
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
@@ -3855,7 +3902,7 @@
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -3865,7 +3912,7 @@
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -3875,7 +3922,7 @@
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
@@ -3885,7 +3932,7 @@
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
@@ -3895,7 +3942,7 @@
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
@@ -3905,7 +3952,7 @@
       <c r="H27" s="6"/>
       <c r="I27" s="6"/>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
@@ -3915,7 +3962,7 @@
       <c r="H28" s="6"/>
       <c r="I28" s="6"/>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
@@ -3925,7 +3972,7 @@
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
@@ -3935,7 +3982,7 @@
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
@@ -3945,7 +3992,7 @@
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -3955,7 +4002,7 @@
       <c r="H32" s="6"/>
       <c r="I32" s="6"/>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
@@ -3965,7 +4012,7 @@
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -3975,7 +4022,7 @@
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
@@ -3985,7 +4032,7 @@
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
@@ -3995,7 +4042,7 @@
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
@@ -4005,7 +4052,7 @@
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
@@ -4015,7 +4062,7 @@
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
@@ -4025,7 +4072,7 @@
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
@@ -4035,7 +4082,7 @@
       <c r="H40" s="6"/>
       <c r="I40" s="6"/>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
@@ -4045,7 +4092,7 @@
       <c r="H41" s="6"/>
       <c r="I41" s="6"/>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
@@ -4055,7 +4102,7 @@
       <c r="H42" s="6"/>
       <c r="I42" s="6"/>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
@@ -4065,7 +4112,7 @@
       <c r="H43" s="6"/>
       <c r="I43" s="6"/>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
@@ -4075,7 +4122,7 @@
       <c r="H44" s="6"/>
       <c r="I44" s="6"/>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
@@ -4085,7 +4132,7 @@
       <c r="H45" s="6"/>
       <c r="I45" s="6"/>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
@@ -4095,7 +4142,7 @@
       <c r="H46" s="6"/>
       <c r="I46" s="6"/>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
@@ -4105,7 +4152,7 @@
       <c r="H47" s="6"/>
       <c r="I47" s="6"/>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
@@ -4115,7 +4162,7 @@
       <c r="H48" s="6"/>
       <c r="I48" s="6"/>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
@@ -4125,7 +4172,7 @@
       <c r="H49" s="6"/>
       <c r="I49" s="6"/>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
@@ -4135,7 +4182,7 @@
       <c r="H50" s="6"/>
       <c r="I50" s="6"/>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
@@ -4145,7 +4192,7 @@
       <c r="H51" s="6"/>
       <c r="I51" s="6"/>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
@@ -4155,7 +4202,7 @@
       <c r="H52" s="6"/>
       <c r="I52" s="6"/>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
@@ -4165,7 +4212,7 @@
       <c r="H53" s="6"/>
       <c r="I53" s="6"/>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
@@ -4175,7 +4222,7 @@
       <c r="H54" s="6"/>
       <c r="I54" s="6"/>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
@@ -4185,7 +4232,7 @@
       <c r="H55" s="6"/>
       <c r="I55" s="6"/>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
@@ -4195,7 +4242,7 @@
       <c r="H56" s="6"/>
       <c r="I56" s="6"/>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
@@ -4205,7 +4252,7 @@
       <c r="H57" s="6"/>
       <c r="I57" s="6"/>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
@@ -4215,7 +4262,7 @@
       <c r="H58" s="6"/>
       <c r="I58" s="6"/>
     </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
       <c r="D59" s="5"/>
@@ -4225,7 +4272,7 @@
       <c r="H59" s="6"/>
       <c r="I59" s="6"/>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
@@ -4235,7 +4282,7 @@
       <c r="H60" s="6"/>
       <c r="I60" s="6"/>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
@@ -4245,7 +4292,7 @@
       <c r="H61" s="6"/>
       <c r="I61" s="6"/>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
@@ -4255,7 +4302,7 @@
       <c r="H62" s="6"/>
       <c r="I62" s="6"/>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
@@ -4265,7 +4312,7 @@
       <c r="H63" s="6"/>
       <c r="I63" s="6"/>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
@@ -4275,7 +4322,7 @@
       <c r="H64" s="6"/>
       <c r="I64" s="6"/>
     </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B65" s="5"/>
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
@@ -4285,7 +4332,7 @@
       <c r="H65" s="6"/>
       <c r="I65" s="6"/>
     </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
@@ -4295,7 +4342,7 @@
       <c r="H66" s="6"/>
       <c r="I66" s="6"/>
     </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
       <c r="D67" s="5"/>
@@ -4305,7 +4352,7 @@
       <c r="H67" s="6"/>
       <c r="I67" s="6"/>
     </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
@@ -4315,7 +4362,7 @@
       <c r="H68" s="6"/>
       <c r="I68" s="6"/>
     </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B69" s="5"/>
       <c r="C69" s="5"/>
       <c r="D69" s="5"/>
@@ -4325,7 +4372,7 @@
       <c r="H69" s="6"/>
       <c r="I69" s="6"/>
     </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B70" s="5"/>
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
@@ -4335,7 +4382,7 @@
       <c r="H70" s="6"/>
       <c r="I70" s="6"/>
     </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B71" s="5"/>
       <c r="C71" s="5"/>
       <c r="D71" s="5"/>
@@ -4345,7 +4392,7 @@
       <c r="H71" s="6"/>
       <c r="I71" s="6"/>
     </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
@@ -4355,7 +4402,7 @@
       <c r="H72" s="6"/>
       <c r="I72" s="6"/>
     </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B73" s="5"/>
       <c r="C73" s="5"/>
       <c r="D73" s="5"/>
@@ -4365,7 +4412,7 @@
       <c r="H73" s="6"/>
       <c r="I73" s="6"/>
     </row>
-    <row r="74" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B74" s="5"/>
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
@@ -4375,7 +4422,7 @@
       <c r="H74" s="6"/>
       <c r="I74" s="6"/>
     </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B75" s="5"/>
       <c r="C75" s="5"/>
       <c r="D75" s="5"/>
@@ -4385,7 +4432,7 @@
       <c r="H75" s="6"/>
       <c r="I75" s="6"/>
     </row>
-    <row r="76" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B76" s="5"/>
       <c r="C76" s="5"/>
       <c r="D76" s="5"/>
@@ -4395,7 +4442,7 @@
       <c r="H76" s="6"/>
       <c r="I76" s="6"/>
     </row>
-    <row r="77" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B77" s="5"/>
       <c r="C77" s="5"/>
       <c r="D77" s="5"/>
@@ -4405,7 +4452,7 @@
       <c r="H77" s="6"/>
       <c r="I77" s="6"/>
     </row>
-    <row r="78" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B78" s="5"/>
       <c r="C78" s="5"/>
       <c r="D78" s="5"/>
@@ -4415,7 +4462,7 @@
       <c r="H78" s="6"/>
       <c r="I78" s="6"/>
     </row>
-    <row r="79" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B79" s="5"/>
       <c r="C79" s="5"/>
       <c r="D79" s="5"/>
@@ -4425,7 +4472,7 @@
       <c r="H79" s="6"/>
       <c r="I79" s="6"/>
     </row>
-    <row r="80" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B80" s="5"/>
       <c r="C80" s="5"/>
       <c r="D80" s="5"/>
@@ -4435,7 +4482,7 @@
       <c r="H80" s="6"/>
       <c r="I80" s="6"/>
     </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B81" s="5"/>
       <c r="C81" s="5"/>
       <c r="D81" s="5"/>
@@ -4445,7 +4492,7 @@
       <c r="H81" s="6"/>
       <c r="I81" s="6"/>
     </row>
-    <row r="82" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B82" s="5"/>
       <c r="C82" s="5"/>
       <c r="D82" s="5"/>
@@ -4455,7 +4502,7 @@
       <c r="H82" s="6"/>
       <c r="I82" s="6"/>
     </row>
-    <row r="83" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B83" s="5"/>
       <c r="C83" s="5"/>
       <c r="D83" s="5"/>
@@ -4465,7 +4512,7 @@
       <c r="H83" s="6"/>
       <c r="I83" s="6"/>
     </row>
-    <row r="84" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B84" s="5"/>
       <c r="C84" s="5"/>
       <c r="D84" s="5"/>
@@ -4475,7 +4522,7 @@
       <c r="H84" s="6"/>
       <c r="I84" s="6"/>
     </row>
-    <row r="85" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B85" s="5"/>
       <c r="C85" s="5"/>
       <c r="D85" s="5"/>
@@ -4485,7 +4532,7 @@
       <c r="H85" s="6"/>
       <c r="I85" s="6"/>
     </row>
-    <row r="86" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
       <c r="D86" s="5"/>
@@ -4495,7 +4542,7 @@
       <c r="H86" s="6"/>
       <c r="I86" s="6"/>
     </row>
-    <row r="87" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B87" s="5"/>
       <c r="C87" s="5"/>
       <c r="D87" s="5"/>
@@ -4505,7 +4552,7 @@
       <c r="H87" s="6"/>
       <c r="I87" s="6"/>
     </row>
-    <row r="88" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B88" s="5"/>
       <c r="C88" s="5"/>
       <c r="D88" s="5"/>
@@ -4515,7 +4562,7 @@
       <c r="H88" s="6"/>
       <c r="I88" s="6"/>
     </row>
-    <row r="89" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B89" s="5"/>
       <c r="C89" s="5"/>
       <c r="D89" s="5"/>
@@ -4525,7 +4572,7 @@
       <c r="H89" s="6"/>
       <c r="I89" s="6"/>
     </row>
-    <row r="90" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B90" s="5"/>
       <c r="C90" s="5"/>
       <c r="D90" s="5"/>
@@ -4535,7 +4582,7 @@
       <c r="H90" s="6"/>
       <c r="I90" s="6"/>
     </row>
-    <row r="91" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B91" s="5"/>
       <c r="C91" s="5"/>
       <c r="D91" s="5"/>
@@ -4545,7 +4592,7 @@
       <c r="H91" s="6"/>
       <c r="I91" s="6"/>
     </row>
-    <row r="92" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B92" s="5"/>
       <c r="C92" s="5"/>
       <c r="D92" s="5"/>
@@ -4555,7 +4602,7 @@
       <c r="H92" s="6"/>
       <c r="I92" s="6"/>
     </row>
-    <row r="93" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B93" s="5"/>
       <c r="C93" s="5"/>
       <c r="D93" s="5"/>
@@ -4565,7 +4612,7 @@
       <c r="H93" s="6"/>
       <c r="I93" s="6"/>
     </row>
-    <row r="94" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B94" s="5"/>
       <c r="C94" s="5"/>
       <c r="D94" s="5"/>
@@ -4575,7 +4622,7 @@
       <c r="H94" s="6"/>
       <c r="I94" s="6"/>
     </row>
-    <row r="95" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B95" s="5"/>
       <c r="C95" s="5"/>
       <c r="D95" s="5"/>
@@ -4585,7 +4632,7 @@
       <c r="H95" s="6"/>
       <c r="I95" s="6"/>
     </row>
-    <row r="96" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B96" s="5"/>
       <c r="C96" s="5"/>
       <c r="D96" s="5"/>
@@ -4595,7 +4642,7 @@
       <c r="H96" s="6"/>
       <c r="I96" s="6"/>
     </row>
-    <row r="97" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B97" s="5"/>
       <c r="C97" s="5"/>
       <c r="D97" s="5"/>
@@ -4605,7 +4652,7 @@
       <c r="H97" s="6"/>
       <c r="I97" s="6"/>
     </row>
-    <row r="98" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B98" s="5"/>
       <c r="C98" s="5"/>
       <c r="D98" s="5"/>
@@ -4615,7 +4662,7 @@
       <c r="H98" s="6"/>
       <c r="I98" s="6"/>
     </row>
-    <row r="99" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="99" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B99" s="5"/>
       <c r="C99" s="5"/>
       <c r="D99" s="5"/>
@@ -4625,7 +4672,7 @@
       <c r="H99" s="6"/>
       <c r="I99" s="6"/>
     </row>
-    <row r="100" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B100" s="5"/>
       <c r="C100" s="5"/>
       <c r="D100" s="5"/>
@@ -4635,7 +4682,7 @@
       <c r="H100" s="6"/>
       <c r="I100" s="6"/>
     </row>
-    <row r="101" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B101" s="5"/>
       <c r="C101" s="5"/>
       <c r="D101" s="5"/>
@@ -4645,7 +4692,7 @@
       <c r="H101" s="6"/>
       <c r="I101" s="6"/>
     </row>
-    <row r="102" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B102" s="5"/>
       <c r="C102" s="5"/>
       <c r="D102" s="5"/>
@@ -4655,7 +4702,7 @@
       <c r="H102" s="6"/>
       <c r="I102" s="6"/>
     </row>
-    <row r="103" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="103" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B103" s="5"/>
       <c r="C103" s="5"/>
       <c r="D103" s="5"/>
@@ -4665,7 +4712,7 @@
       <c r="H103" s="6"/>
       <c r="I103" s="6"/>
     </row>
-    <row r="104" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B104" s="5"/>
       <c r="C104" s="5"/>
       <c r="D104" s="5"/>
@@ -4675,7 +4722,7 @@
       <c r="H104" s="6"/>
       <c r="I104" s="6"/>
     </row>
-    <row r="105" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B105" s="5"/>
       <c r="C105" s="5"/>
       <c r="D105" s="5"/>
@@ -4685,7 +4732,7 @@
       <c r="H105" s="6"/>
       <c r="I105" s="6"/>
     </row>
-    <row r="106" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B106" s="5"/>
       <c r="C106" s="5"/>
       <c r="D106" s="5"/>
@@ -4695,7 +4742,7 @@
       <c r="H106" s="6"/>
       <c r="I106" s="6"/>
     </row>
-    <row r="107" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B107" s="5"/>
       <c r="C107" s="5"/>
       <c r="D107" s="5"/>
@@ -4705,7 +4752,7 @@
       <c r="H107" s="6"/>
       <c r="I107" s="6"/>
     </row>
-    <row r="108" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B108" s="5"/>
       <c r="C108" s="5"/>
       <c r="D108" s="5"/>
@@ -4715,7 +4762,7 @@
       <c r="H108" s="6"/>
       <c r="I108" s="6"/>
     </row>
-    <row r="109" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B109" s="5"/>
       <c r="C109" s="5"/>
       <c r="D109" s="5"/>
@@ -4725,7 +4772,7 @@
       <c r="H109" s="6"/>
       <c r="I109" s="6"/>
     </row>
-    <row r="110" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="110" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B110" s="5"/>
       <c r="C110" s="5"/>
       <c r="D110" s="5"/>
@@ -4735,7 +4782,7 @@
       <c r="H110" s="6"/>
       <c r="I110" s="6"/>
     </row>
-    <row r="111" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="111" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B111" s="5"/>
       <c r="C111" s="5"/>
       <c r="D111" s="5"/>
@@ -4745,7 +4792,7 @@
       <c r="H111" s="6"/>
       <c r="I111" s="6"/>
     </row>
-    <row r="112" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="112" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B112" s="5"/>
       <c r="C112" s="5"/>
       <c r="D112" s="5"/>
@@ -4755,7 +4802,7 @@
       <c r="H112" s="6"/>
       <c r="I112" s="6"/>
     </row>
-    <row r="113" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="113" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B113" s="5"/>
       <c r="C113" s="5"/>
       <c r="D113" s="5"/>
@@ -4765,7 +4812,7 @@
       <c r="H113" s="6"/>
       <c r="I113" s="6"/>
     </row>
-    <row r="114" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="114" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B114" s="5"/>
       <c r="C114" s="5"/>
       <c r="D114" s="5"/>
@@ -4775,7 +4822,7 @@
       <c r="H114" s="6"/>
       <c r="I114" s="6"/>
     </row>
-    <row r="115" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="115" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B115" s="5"/>
       <c r="C115" s="5"/>
       <c r="D115" s="5"/>
@@ -4785,7 +4832,7 @@
       <c r="H115" s="6"/>
       <c r="I115" s="6"/>
     </row>
-    <row r="116" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="116" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B116" s="5"/>
       <c r="C116" s="5"/>
       <c r="D116" s="5"/>
@@ -4795,7 +4842,7 @@
       <c r="H116" s="6"/>
       <c r="I116" s="6"/>
     </row>
-    <row r="117" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="117" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B117" s="5"/>
       <c r="C117" s="5"/>
       <c r="D117" s="5"/>
@@ -4805,7 +4852,7 @@
       <c r="H117" s="6"/>
       <c r="I117" s="6"/>
     </row>
-    <row r="118" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="118" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B118" s="5"/>
       <c r="C118" s="5"/>
       <c r="D118" s="5"/>
@@ -4815,7 +4862,7 @@
       <c r="H118" s="6"/>
       <c r="I118" s="6"/>
     </row>
-    <row r="119" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="119" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B119" s="5"/>
       <c r="C119" s="5"/>
       <c r="D119" s="5"/>
@@ -4825,7 +4872,7 @@
       <c r="H119" s="6"/>
       <c r="I119" s="6"/>
     </row>
-    <row r="120" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="120" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B120" s="5"/>
       <c r="C120" s="5"/>
       <c r="D120" s="5"/>
@@ -4835,7 +4882,7 @@
       <c r="H120" s="6"/>
       <c r="I120" s="6"/>
     </row>
-    <row r="121" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="121" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B121" s="5"/>
       <c r="C121" s="5"/>
       <c r="D121" s="5"/>
@@ -4845,7 +4892,7 @@
       <c r="H121" s="6"/>
       <c r="I121" s="6"/>
     </row>
-    <row r="122" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="122" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B122" s="5"/>
       <c r="C122" s="5"/>
       <c r="D122" s="5"/>
@@ -4855,7 +4902,7 @@
       <c r="H122" s="6"/>
       <c r="I122" s="6"/>
     </row>
-    <row r="123" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="123" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B123" s="5"/>
       <c r="C123" s="5"/>
       <c r="D123" s="5"/>
@@ -4865,7 +4912,7 @@
       <c r="H123" s="6"/>
       <c r="I123" s="6"/>
     </row>
-    <row r="124" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="124" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B124" s="5"/>
       <c r="C124" s="5"/>
       <c r="D124" s="5"/>
@@ -4875,7 +4922,7 @@
       <c r="H124" s="6"/>
       <c r="I124" s="6"/>
     </row>
-    <row r="125" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="125" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B125" s="5"/>
       <c r="C125" s="5"/>
       <c r="D125" s="5"/>
@@ -4885,7 +4932,7 @@
       <c r="H125" s="6"/>
       <c r="I125" s="6"/>
     </row>
-    <row r="126" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="126" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B126" s="5"/>
       <c r="C126" s="5"/>
       <c r="D126" s="5"/>
@@ -4895,7 +4942,7 @@
       <c r="H126" s="6"/>
       <c r="I126" s="6"/>
     </row>
-    <row r="127" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="127" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B127" s="5"/>
       <c r="C127" s="5"/>
       <c r="D127" s="5"/>
@@ -4905,7 +4952,7 @@
       <c r="H127" s="6"/>
       <c r="I127" s="6"/>
     </row>
-    <row r="128" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="128" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B128" s="5"/>
       <c r="C128" s="5"/>
       <c r="D128" s="5"/>
@@ -4915,7 +4962,7 @@
       <c r="H128" s="6"/>
       <c r="I128" s="6"/>
     </row>
-    <row r="129" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="129" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B129" s="5"/>
       <c r="C129" s="5"/>
       <c r="D129" s="5"/>
@@ -4925,7 +4972,7 @@
       <c r="H129" s="6"/>
       <c r="I129" s="6"/>
     </row>
-    <row r="130" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="130" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B130" s="5"/>
       <c r="C130" s="5"/>
       <c r="D130" s="5"/>
@@ -4935,7 +4982,7 @@
       <c r="H130" s="6"/>
       <c r="I130" s="6"/>
     </row>
-    <row r="131" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="131" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B131" s="5"/>
       <c r="C131" s="5"/>
       <c r="D131" s="5"/>
@@ -4945,7 +4992,7 @@
       <c r="H131" s="6"/>
       <c r="I131" s="6"/>
     </row>
-    <row r="132" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="132" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B132" s="5"/>
       <c r="C132" s="5"/>
       <c r="D132" s="5"/>
@@ -4955,7 +5002,7 @@
       <c r="H132" s="6"/>
       <c r="I132" s="6"/>
     </row>
-    <row r="133" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="133" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B133" s="5"/>
       <c r="C133" s="5"/>
       <c r="D133" s="5"/>
@@ -4965,7 +5012,7 @@
       <c r="H133" s="6"/>
       <c r="I133" s="6"/>
     </row>
-    <row r="134" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="134" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B134" s="5"/>
       <c r="C134" s="5"/>
       <c r="D134" s="5"/>
@@ -4975,7 +5022,7 @@
       <c r="H134" s="6"/>
       <c r="I134" s="6"/>
     </row>
-    <row r="135" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="135" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B135" s="5"/>
       <c r="C135" s="5"/>
       <c r="D135" s="5"/>
@@ -4985,7 +5032,7 @@
       <c r="H135" s="6"/>
       <c r="I135" s="6"/>
     </row>
-    <row r="136" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="136" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B136" s="5"/>
       <c r="C136" s="5"/>
       <c r="D136" s="5"/>
@@ -4995,7 +5042,7 @@
       <c r="H136" s="6"/>
       <c r="I136" s="6"/>
     </row>
-    <row r="137" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="137" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B137" s="5"/>
       <c r="C137" s="5"/>
       <c r="D137" s="5"/>
@@ -5005,7 +5052,7 @@
       <c r="H137" s="6"/>
       <c r="I137" s="6"/>
     </row>
-    <row r="138" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="138" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B138" s="5"/>
       <c r="C138" s="5"/>
       <c r="D138" s="5"/>
@@ -5015,7 +5062,7 @@
       <c r="H138" s="6"/>
       <c r="I138" s="6"/>
     </row>
-    <row r="139" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="139" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B139" s="5"/>
       <c r="C139" s="5"/>
       <c r="D139" s="5"/>
@@ -5025,7 +5072,7 @@
       <c r="H139" s="6"/>
       <c r="I139" s="6"/>
     </row>
-    <row r="140" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="140" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B140" s="5"/>
       <c r="C140" s="5"/>
       <c r="D140" s="5"/>
@@ -5035,7 +5082,7 @@
       <c r="H140" s="6"/>
       <c r="I140" s="6"/>
     </row>
-    <row r="141" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="141" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B141" s="5"/>
       <c r="C141" s="5"/>
       <c r="D141" s="5"/>
@@ -5045,7 +5092,7 @@
       <c r="H141" s="6"/>
       <c r="I141" s="6"/>
     </row>
-    <row r="142" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="142" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B142" s="5"/>
       <c r="C142" s="5"/>
       <c r="D142" s="5"/>
@@ -5055,7 +5102,7 @@
       <c r="H142" s="6"/>
       <c r="I142" s="6"/>
     </row>
-    <row r="143" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="143" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B143" s="5"/>
       <c r="C143" s="5"/>
       <c r="D143" s="5"/>
@@ -5065,7 +5112,7 @@
       <c r="H143" s="6"/>
       <c r="I143" s="6"/>
     </row>
-    <row r="144" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="144" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B144" s="5"/>
       <c r="C144" s="5"/>
       <c r="D144" s="5"/>
@@ -5075,7 +5122,7 @@
       <c r="H144" s="6"/>
       <c r="I144" s="6"/>
     </row>
-    <row r="145" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="145" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B145" s="5"/>
       <c r="C145" s="5"/>
       <c r="D145" s="5"/>
@@ -5085,7 +5132,7 @@
       <c r="H145" s="6"/>
       <c r="I145" s="6"/>
     </row>
-    <row r="146" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="146" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B146" s="5"/>
       <c r="C146" s="5"/>
       <c r="D146" s="5"/>
@@ -5095,7 +5142,7 @@
       <c r="H146" s="6"/>
       <c r="I146" s="6"/>
     </row>
-    <row r="147" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="147" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B147" s="5"/>
       <c r="C147" s="5"/>
       <c r="D147" s="5"/>
@@ -5105,7 +5152,7 @@
       <c r="H147" s="6"/>
       <c r="I147" s="6"/>
     </row>
-    <row r="148" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="148" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B148" s="5"/>
       <c r="C148" s="5"/>
       <c r="D148" s="5"/>
@@ -5115,7 +5162,7 @@
       <c r="H148" s="6"/>
       <c r="I148" s="6"/>
     </row>
-    <row r="149" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="149" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B149" s="5"/>
       <c r="C149" s="5"/>
       <c r="D149" s="5"/>
@@ -5125,7 +5172,7 @@
       <c r="H149" s="6"/>
       <c r="I149" s="6"/>
     </row>
-    <row r="150" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="150" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B150" s="5"/>
       <c r="C150" s="5"/>
       <c r="D150" s="5"/>
@@ -5135,7 +5182,7 @@
       <c r="H150" s="6"/>
       <c r="I150" s="6"/>
     </row>
-    <row r="151" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="151" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B151" s="5"/>
       <c r="C151" s="5"/>
       <c r="D151" s="5"/>
@@ -5145,7 +5192,7 @@
       <c r="H151" s="6"/>
       <c r="I151" s="6"/>
     </row>
-    <row r="152" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="152" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B152" s="5"/>
       <c r="C152" s="5"/>
       <c r="D152" s="5"/>
@@ -5155,7 +5202,7 @@
       <c r="H152" s="6"/>
       <c r="I152" s="6"/>
     </row>
-    <row r="153" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="153" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B153" s="5"/>
       <c r="C153" s="5"/>
       <c r="D153" s="5"/>
@@ -5165,7 +5212,7 @@
       <c r="H153" s="6"/>
       <c r="I153" s="6"/>
     </row>
-    <row r="154" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="154" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B154" s="5"/>
       <c r="C154" s="5"/>
       <c r="D154" s="5"/>
@@ -5175,7 +5222,7 @@
       <c r="H154" s="6"/>
       <c r="I154" s="6"/>
     </row>
-    <row r="155" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="155" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B155" s="5"/>
       <c r="C155" s="5"/>
       <c r="D155" s="5"/>
@@ -5185,7 +5232,7 @@
       <c r="H155" s="6"/>
       <c r="I155" s="6"/>
     </row>
-    <row r="156" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="156" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B156" s="5"/>
       <c r="C156" s="5"/>
       <c r="D156" s="5"/>
@@ -5195,7 +5242,7 @@
       <c r="H156" s="6"/>
       <c r="I156" s="6"/>
     </row>
-    <row r="157" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="157" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B157" s="5"/>
       <c r="C157" s="5"/>
       <c r="D157" s="5"/>
@@ -5205,7 +5252,7 @@
       <c r="H157" s="6"/>
       <c r="I157" s="6"/>
     </row>
-    <row r="158" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="158" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B158" s="5"/>
       <c r="C158" s="5"/>
       <c r="D158" s="5"/>
@@ -5215,7 +5262,7 @@
       <c r="H158" s="6"/>
       <c r="I158" s="6"/>
     </row>
-    <row r="159" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="159" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B159" s="5"/>
       <c r="C159" s="5"/>
       <c r="D159" s="5"/>
@@ -5225,7 +5272,7 @@
       <c r="H159" s="6"/>
       <c r="I159" s="6"/>
     </row>
-    <row r="160" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="160" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B160" s="5"/>
       <c r="C160" s="5"/>
       <c r="D160" s="5"/>
@@ -5235,7 +5282,7 @@
       <c r="H160" s="6"/>
       <c r="I160" s="6"/>
     </row>
-    <row r="161" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="161" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B161" s="5"/>
       <c r="C161" s="5"/>
       <c r="D161" s="5"/>
@@ -5245,7 +5292,7 @@
       <c r="H161" s="6"/>
       <c r="I161" s="6"/>
     </row>
-    <row r="162" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="162" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B162" s="5"/>
       <c r="C162" s="5"/>
       <c r="D162" s="5"/>
@@ -5255,7 +5302,7 @@
       <c r="H162" s="6"/>
       <c r="I162" s="6"/>
     </row>
-    <row r="163" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="163" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B163" s="5"/>
       <c r="C163" s="5"/>
       <c r="D163" s="5"/>
@@ -5265,7 +5312,7 @@
       <c r="H163" s="6"/>
       <c r="I163" s="6"/>
     </row>
-    <row r="164" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="164" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B164" s="5"/>
       <c r="C164" s="5"/>
       <c r="D164" s="5"/>
@@ -5275,7 +5322,7 @@
       <c r="H164" s="6"/>
       <c r="I164" s="6"/>
     </row>
-    <row r="165" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="165" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B165" s="5"/>
       <c r="C165" s="5"/>
       <c r="D165" s="5"/>
@@ -5285,7 +5332,7 @@
       <c r="H165" s="6"/>
       <c r="I165" s="6"/>
     </row>
-    <row r="166" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="166" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B166" s="5"/>
       <c r="C166" s="5"/>
       <c r="D166" s="5"/>
@@ -5295,7 +5342,7 @@
       <c r="H166" s="6"/>
       <c r="I166" s="6"/>
     </row>
-    <row r="167" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="167" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B167" s="5"/>
       <c r="C167" s="5"/>
       <c r="D167" s="5"/>
@@ -5305,7 +5352,7 @@
       <c r="H167" s="6"/>
       <c r="I167" s="6"/>
     </row>
-    <row r="168" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="168" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B168" s="5"/>
       <c r="C168" s="5"/>
       <c r="D168" s="5"/>
@@ -5315,7 +5362,7 @@
       <c r="H168" s="6"/>
       <c r="I168" s="6"/>
     </row>
-    <row r="169" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="169" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B169" s="5"/>
       <c r="C169" s="5"/>
       <c r="D169" s="5"/>
@@ -5325,7 +5372,7 @@
       <c r="H169" s="6"/>
       <c r="I169" s="6"/>
     </row>
-    <row r="170" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="170" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B170" s="5"/>
       <c r="C170" s="5"/>
       <c r="D170" s="5"/>
@@ -5335,7 +5382,7 @@
       <c r="H170" s="6"/>
       <c r="I170" s="6"/>
     </row>
-    <row r="171" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="171" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B171" s="5"/>
       <c r="C171" s="5"/>
       <c r="D171" s="5"/>
@@ -5345,7 +5392,7 @@
       <c r="H171" s="6"/>
       <c r="I171" s="6"/>
     </row>
-    <row r="172" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="172" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B172" s="5"/>
       <c r="C172" s="5"/>
       <c r="D172" s="5"/>
@@ -5355,7 +5402,7 @@
       <c r="H172" s="6"/>
       <c r="I172" s="6"/>
     </row>
-    <row r="173" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="173" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B173" s="5"/>
       <c r="C173" s="5"/>
       <c r="D173" s="5"/>
@@ -5365,7 +5412,7 @@
       <c r="H173" s="6"/>
       <c r="I173" s="6"/>
     </row>
-    <row r="174" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="174" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B174" s="5"/>
       <c r="C174" s="5"/>
       <c r="D174" s="5"/>
@@ -5375,7 +5422,7 @@
       <c r="H174" s="6"/>
       <c r="I174" s="6"/>
     </row>
-    <row r="175" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="175" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B175" s="5"/>
       <c r="C175" s="5"/>
       <c r="D175" s="5"/>
@@ -5385,7 +5432,7 @@
       <c r="H175" s="6"/>
       <c r="I175" s="6"/>
     </row>
-    <row r="176" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="176" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B176" s="5"/>
       <c r="C176" s="5"/>
       <c r="D176" s="5"/>
@@ -5395,7 +5442,7 @@
       <c r="H176" s="6"/>
       <c r="I176" s="6"/>
     </row>
-    <row r="177" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="177" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B177" s="5"/>
       <c r="C177" s="5"/>
       <c r="D177" s="5"/>
@@ -5405,7 +5452,7 @@
       <c r="H177" s="6"/>
       <c r="I177" s="6"/>
     </row>
-    <row r="178" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="178" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B178" s="5"/>
       <c r="C178" s="5"/>
       <c r="D178" s="5"/>
@@ -5415,7 +5462,7 @@
       <c r="H178" s="6"/>
       <c r="I178" s="6"/>
     </row>
-    <row r="179" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="179" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B179" s="5"/>
       <c r="C179" s="5"/>
       <c r="D179" s="5"/>
@@ -5425,7 +5472,7 @@
       <c r="H179" s="6"/>
       <c r="I179" s="6"/>
     </row>
-    <row r="180" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="180" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B180" s="5"/>
       <c r="C180" s="5"/>
       <c r="D180" s="5"/>
@@ -5435,7 +5482,7 @@
       <c r="H180" s="6"/>
       <c r="I180" s="6"/>
     </row>
-    <row r="181" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="181" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B181" s="5"/>
       <c r="C181" s="5"/>
       <c r="D181" s="5"/>
@@ -5445,7 +5492,7 @@
       <c r="H181" s="6"/>
       <c r="I181" s="6"/>
     </row>
-    <row r="182" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="182" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B182" s="5"/>
       <c r="C182" s="5"/>
       <c r="D182" s="5"/>
@@ -5455,7 +5502,7 @@
       <c r="H182" s="6"/>
       <c r="I182" s="6"/>
     </row>
-    <row r="183" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="183" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B183" s="5"/>
       <c r="C183" s="5"/>
       <c r="D183" s="5"/>
@@ -5465,7 +5512,7 @@
       <c r="H183" s="6"/>
       <c r="I183" s="6"/>
     </row>
-    <row r="184" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="184" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B184" s="5"/>
       <c r="C184" s="5"/>
       <c r="D184" s="5"/>
@@ -5475,7 +5522,7 @@
       <c r="H184" s="6"/>
       <c r="I184" s="6"/>
     </row>
-    <row r="185" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="185" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B185" s="5"/>
       <c r="C185" s="5"/>
       <c r="D185" s="5"/>
@@ -5485,7 +5532,7 @@
       <c r="H185" s="6"/>
       <c r="I185" s="6"/>
     </row>
-    <row r="186" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="186" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B186" s="5"/>
       <c r="C186" s="5"/>
       <c r="D186" s="5"/>
@@ -5495,7 +5542,7 @@
       <c r="H186" s="6"/>
       <c r="I186" s="6"/>
     </row>
-    <row r="187" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="187" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B187" s="5"/>
       <c r="C187" s="5"/>
       <c r="D187" s="5"/>
@@ -5505,7 +5552,7 @@
       <c r="H187" s="6"/>
       <c r="I187" s="6"/>
     </row>
-    <row r="188" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="188" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B188" s="5"/>
       <c r="C188" s="5"/>
       <c r="D188" s="5"/>
@@ -5515,7 +5562,7 @@
       <c r="H188" s="6"/>
       <c r="I188" s="6"/>
     </row>
-    <row r="189" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="189" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B189" s="5"/>
       <c r="C189" s="5"/>
       <c r="D189" s="5"/>
@@ -5525,7 +5572,7 @@
       <c r="H189" s="6"/>
       <c r="I189" s="6"/>
     </row>
-    <row r="190" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="190" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B190" s="5"/>
       <c r="C190" s="5"/>
       <c r="D190" s="5"/>
@@ -5535,7 +5582,7 @@
       <c r="H190" s="6"/>
       <c r="I190" s="6"/>
     </row>
-    <row r="191" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="191" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B191" s="5"/>
       <c r="C191" s="5"/>
       <c r="D191" s="5"/>
@@ -5545,7 +5592,7 @@
       <c r="H191" s="6"/>
       <c r="I191" s="6"/>
     </row>
-    <row r="192" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="192" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B192" s="5"/>
       <c r="C192" s="5"/>
       <c r="D192" s="5"/>
@@ -5555,7 +5602,7 @@
       <c r="H192" s="6"/>
       <c r="I192" s="6"/>
     </row>
-    <row r="193" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="193" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B193" s="5"/>
       <c r="C193" s="5"/>
       <c r="D193" s="5"/>
@@ -5565,7 +5612,7 @@
       <c r="H193" s="6"/>
       <c r="I193" s="6"/>
     </row>
-    <row r="194" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="194" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B194" s="5"/>
       <c r="C194" s="5"/>
       <c r="D194" s="5"/>
@@ -5575,7 +5622,7 @@
       <c r="H194" s="6"/>
       <c r="I194" s="6"/>
     </row>
-    <row r="195" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="195" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B195" s="5"/>
       <c r="C195" s="5"/>
       <c r="D195" s="5"/>
@@ -5585,7 +5632,7 @@
       <c r="H195" s="6"/>
       <c r="I195" s="6"/>
     </row>
-    <row r="196" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="196" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B196" s="5"/>
       <c r="C196" s="5"/>
       <c r="D196" s="5"/>
@@ -5595,7 +5642,7 @@
       <c r="H196" s="6"/>
       <c r="I196" s="6"/>
     </row>
-    <row r="197" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="197" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B197" s="5"/>
       <c r="C197" s="5"/>
       <c r="D197" s="5"/>
@@ -5605,7 +5652,7 @@
       <c r="H197" s="6"/>
       <c r="I197" s="6"/>
     </row>
-    <row r="198" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="198" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B198" s="5"/>
       <c r="C198" s="5"/>
       <c r="D198" s="5"/>
@@ -5615,7 +5662,7 @@
       <c r="H198" s="6"/>
       <c r="I198" s="6"/>
     </row>
-    <row r="199" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="199" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B199" s="5"/>
       <c r="C199" s="5"/>
       <c r="D199" s="5"/>
@@ -5625,7 +5672,7 @@
       <c r="H199" s="6"/>
       <c r="I199" s="6"/>
     </row>
-    <row r="200" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="200" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B200" s="5"/>
       <c r="C200" s="5"/>
       <c r="D200" s="5"/>

</xml_diff>

<commit_message>
Updated the Pipeline_mod to monitor additional asset types
</commit_message>
<xml_diff>
--- a/Opportunities/Pipeline_monitor/Pipeline_monitor.xlsx
+++ b/Opportunities/Pipeline_monitor/Pipeline_monitor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kamanl/PycharmProjects/Investing_project/Opportunities/Pipeline_monitor/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jerry.chen\PycharmProjects\pythonProject\Opportunities\Pipeline_monitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{427ADB3E-6524-A94C-AE93-FB0ADCB7A7EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E4DE9B2A-44BA-483C-98AD-3EF0DA98755E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="1140" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Monitor" sheetId="1" r:id="rId1"/>
@@ -20,17 +20,14 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Current_Holdings!$B$6:$J$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Monitor!$B$4:$N$4</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
   <si>
     <t>Pipeline Monitor</t>
   </si>
@@ -74,6 +71,15 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>0806.HK</t>
+  </si>
+  <si>
+    <t>VALUE PARTNERS</t>
+  </si>
+  <si>
+    <t>HKG</t>
   </si>
   <si>
     <t>Current Holdings Monitor</t>
@@ -115,19 +121,22 @@
     <t xml:space="preserve">Total Protfolio at FV = </t>
   </si>
   <si>
-    <t>0806.HK</t>
-  </si>
-  <si>
-    <t>VALUE PARTNERS</t>
-  </si>
-  <si>
-    <t>HKG</t>
-  </si>
-  <si>
     <t>1475.HK</t>
   </si>
   <si>
     <t>NISSIN FOODS</t>
+  </si>
+  <si>
+    <t>0697.HK</t>
+  </si>
+  <si>
+    <t>SHOUCHENG</t>
+  </si>
+  <si>
+    <t>3718.HK</t>
+  </si>
+  <si>
+    <t>BJ ENT URBAN</t>
   </si>
   <si>
     <t>603338.SS</t>
@@ -139,16 +148,13 @@
     <t>SHH</t>
   </si>
   <si>
-    <t>3718.HK</t>
+    <t>Park</t>
   </si>
   <si>
-    <t>BJ ENT URBAN</t>
+    <t>Project Park</t>
   </si>
   <si>
-    <t>0697.HK</t>
-  </si>
-  <si>
-    <t>SHOUCHENG</t>
+    <t>Private Credit</t>
   </si>
 </sst>
 </file>
@@ -178,7 +184,6 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -685,19 +690,19 @@
   <dimension ref="A2:N200"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.5" customWidth="1"/>
-    <col min="2" max="11" width="14.6640625" customWidth="1"/>
-    <col min="12" max="12" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.6640625" customWidth="1"/>
-    <col min="14" max="14" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="2.453125" customWidth="1"/>
+    <col min="2" max="11" width="14.6328125" customWidth="1"/>
+    <col min="12" max="12" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.7265625" customWidth="1"/>
+    <col min="14" max="14" width="14.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -715,7 +720,7 @@
       <c r="M2" s="15"/>
       <c r="N2" s="15"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
@@ -738,7 +743,7 @@
         <v>7</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>8</v>
@@ -750,44 +755,44 @@
         <v>10</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B5" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="E5" s="7">
-        <v>0.66</v>
+        <v>1.75</v>
       </c>
       <c r="F5" s="6">
-        <v>1.0970527454262955</v>
+        <v>0.1048451206880141</v>
       </c>
       <c r="G5" s="6">
-        <v>0.19492479482945849</v>
+        <v>9.7869190335055159E-2</v>
       </c>
       <c r="H5" s="6">
         <f>F5-G5</f>
-        <v>0.90212795059683704</v>
+        <v>6.975930352958945E-3</v>
       </c>
       <c r="I5" s="5">
-        <v>0.14560000000000001</v>
+        <v>9.6099999999999991E-2</v>
       </c>
       <c r="J5" s="6">
         <f>I5/E5</f>
-        <v>0.22060606060606061</v>
+        <v>5.4914285714285707E-2</v>
       </c>
       <c r="K5" s="7">
-        <v>5.3</v>
+        <v>1.35</v>
       </c>
       <c r="L5" s="8">
         <v>44925</v>
@@ -796,38 +801,38 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B6" s="5" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="E6" s="7">
-        <v>2.6</v>
+        <v>2.65</v>
       </c>
       <c r="F6" s="6">
-        <v>5.7459512467880058E-2</v>
+        <v>0.29168745104054361</v>
       </c>
       <c r="G6" s="6">
-        <v>9.3811838619443283E-2</v>
+        <v>0.13498782138261814</v>
       </c>
       <c r="H6" s="6">
         <f>F6-G6</f>
-        <v>-3.6352326151563225E-2</v>
+        <v>0.15669962965792547</v>
       </c>
       <c r="I6" s="5">
-        <v>0</v>
+        <v>0.14560000000000001</v>
       </c>
       <c r="J6" s="6">
         <f>I6/E6</f>
-        <v>0</v>
+        <v>5.49433962264151E-2</v>
       </c>
       <c r="K6" s="7">
-        <v>2.12</v>
+        <v>5.3</v>
       </c>
       <c r="L6" s="8">
         <v>44925</v>
@@ -836,7 +841,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B7" s="5" t="s">
         <v>28</v>
       </c>
@@ -844,30 +849,30 @@
         <v>29</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="E7" s="7">
-        <v>6.54</v>
+        <v>6.49</v>
       </c>
       <c r="F7" s="6">
-        <v>4.9815184991756523E-2</v>
+        <v>5.4538697758065524E-2</v>
       </c>
       <c r="G7" s="6">
-        <v>9.7090573713234762E-2</v>
+        <v>0.10888333370903769</v>
       </c>
       <c r="H7" s="6">
         <f>F7-G7</f>
-        <v>-4.727538872147824E-2</v>
+        <v>-5.4344635950972164E-2</v>
       </c>
       <c r="I7" s="5">
         <v>0.14560000000000001</v>
       </c>
       <c r="J7" s="6">
         <f>I7/E7</f>
-        <v>2.2262996941896027E-2</v>
+        <v>2.2434514637904468E-2</v>
       </c>
       <c r="K7" s="7">
-        <v>4.9000000000000004</v>
+        <v>5.3</v>
       </c>
       <c r="L7" s="8">
         <v>45015</v>
@@ -876,101 +881,119 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B8" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="E8" s="7">
-        <v>53.88</v>
+        <v>0.67</v>
       </c>
       <c r="F8" s="6">
-        <v>-0.28739529366053429</v>
+        <v>1.0729011340280459</v>
       </c>
       <c r="G8" s="6">
-        <v>8.167411802127264E-2</v>
+        <v>0.19492479482945849</v>
       </c>
       <c r="H8" s="6">
         <f>F8-G8</f>
-        <v>-0.36906941168180696</v>
+        <v>0.87797633919858742</v>
       </c>
       <c r="I8" s="5">
         <v>0.14560000000000001</v>
       </c>
       <c r="J8" s="6">
         <f>I8/E8</f>
-        <v>2.7023014105419449E-3</v>
+        <v>0.21731343283582089</v>
       </c>
       <c r="K8" s="7">
         <v>5.3</v>
       </c>
       <c r="L8" s="8">
-        <v>45015</v>
+        <v>44925</v>
       </c>
       <c r="M8" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="D9" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>27</v>
-      </c>
       <c r="E9" s="7">
-        <v>1.74</v>
+        <v>51.6</v>
       </c>
       <c r="F9" s="6">
-        <v>-0.25796975571396996</v>
+        <v>-0.27051219688264538</v>
       </c>
       <c r="G9" s="6">
-        <v>0.35888736715901126</v>
+        <v>8.157089286470498E-2</v>
       </c>
       <c r="H9" s="6">
         <f>F9-G9</f>
-        <v>-0.61685712287298122</v>
+        <v>-0.35208308974735036</v>
       </c>
       <c r="I9" s="5">
         <v>0.14560000000000001</v>
       </c>
       <c r="J9" s="6">
         <f>I9/E9</f>
-        <v>8.3678160919540237E-2</v>
+        <v>2.8217054263565892E-3</v>
       </c>
       <c r="K9" s="7">
         <v>5.3</v>
       </c>
       <c r="L9" s="8">
-        <v>44925</v>
+        <v>45015</v>
       </c>
       <c r="M9" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="7"/>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B10" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="7">
+        <v>23880000</v>
+      </c>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
+      <c r="H10" s="6">
+        <f>F10-G10</f>
+        <v>0</v>
+      </c>
       <c r="I10" s="5"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="8"/>
+      <c r="J10" s="6">
+        <f>I10/E10</f>
+        <v>0</v>
+      </c>
+      <c r="K10" s="7">
+        <v>0</v>
+      </c>
+      <c r="L10" s="8">
+        <v>44911</v>
+      </c>
       <c r="M10" s="8"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -984,7 +1007,7 @@
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -998,7 +1021,7 @@
       <c r="L12" s="8"/>
       <c r="M12" s="8"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -1012,7 +1035,7 @@
       <c r="L13" s="8"/>
       <c r="M13" s="8"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -1026,7 +1049,7 @@
       <c r="L14" s="8"/>
       <c r="M14" s="8"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -1040,7 +1063,7 @@
       <c r="L15" s="8"/>
       <c r="M15" s="8"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -1054,7 +1077,7 @@
       <c r="L16" s="8"/>
       <c r="M16" s="8"/>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -1068,7 +1091,7 @@
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -1082,7 +1105,7 @@
       <c r="L18" s="8"/>
       <c r="M18" s="8"/>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -1096,7 +1119,7 @@
       <c r="L19" s="8"/>
       <c r="M19" s="8"/>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
@@ -1110,7 +1133,7 @@
       <c r="L20" s="8"/>
       <c r="M20" s="8"/>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
@@ -1124,7 +1147,7 @@
       <c r="L21" s="8"/>
       <c r="M21" s="8"/>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
@@ -1138,7 +1161,7 @@
       <c r="L22" s="8"/>
       <c r="M22" s="8"/>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -1152,7 +1175,7 @@
       <c r="L23" s="8"/>
       <c r="M23" s="8"/>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -1166,7 +1189,7 @@
       <c r="L24" s="8"/>
       <c r="M24" s="8"/>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
@@ -1180,7 +1203,7 @@
       <c r="L25" s="8"/>
       <c r="M25" s="8"/>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
@@ -1194,7 +1217,7 @@
       <c r="L26" s="8"/>
       <c r="M26" s="8"/>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
@@ -1208,7 +1231,7 @@
       <c r="L27" s="8"/>
       <c r="M27" s="8"/>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
@@ -1222,7 +1245,7 @@
       <c r="L28" s="8"/>
       <c r="M28" s="8"/>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
@@ -1236,7 +1259,7 @@
       <c r="L29" s="8"/>
       <c r="M29" s="8"/>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
@@ -1250,7 +1273,7 @@
       <c r="L30" s="8"/>
       <c r="M30" s="8"/>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
@@ -1264,7 +1287,7 @@
       <c r="L31" s="8"/>
       <c r="M31" s="8"/>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -1278,7 +1301,7 @@
       <c r="L32" s="8"/>
       <c r="M32" s="8"/>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
@@ -1292,7 +1315,7 @@
       <c r="L33" s="8"/>
       <c r="M33" s="8"/>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -1306,7 +1329,7 @@
       <c r="L34" s="8"/>
       <c r="M34" s="8"/>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
@@ -1320,7 +1343,7 @@
       <c r="L35" s="8"/>
       <c r="M35" s="8"/>
     </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
@@ -1334,7 +1357,7 @@
       <c r="L36" s="8"/>
       <c r="M36" s="8"/>
     </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
@@ -1348,7 +1371,7 @@
       <c r="L37" s="8"/>
       <c r="M37" s="8"/>
     </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
@@ -1362,7 +1385,7 @@
       <c r="L38" s="8"/>
       <c r="M38" s="8"/>
     </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
@@ -1376,7 +1399,7 @@
       <c r="L39" s="8"/>
       <c r="M39" s="8"/>
     </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
@@ -1390,7 +1413,7 @@
       <c r="L40" s="8"/>
       <c r="M40" s="8"/>
     </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
@@ -1404,7 +1427,7 @@
       <c r="L41" s="8"/>
       <c r="M41" s="8"/>
     </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
@@ -1418,7 +1441,7 @@
       <c r="L42" s="8"/>
       <c r="M42" s="8"/>
     </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
@@ -1432,7 +1455,7 @@
       <c r="L43" s="8"/>
       <c r="M43" s="8"/>
     </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
@@ -1446,7 +1469,7 @@
       <c r="L44" s="8"/>
       <c r="M44" s="8"/>
     </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
@@ -1460,7 +1483,7 @@
       <c r="L45" s="8"/>
       <c r="M45" s="8"/>
     </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
@@ -1474,7 +1497,7 @@
       <c r="L46" s="8"/>
       <c r="M46" s="8"/>
     </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
@@ -1488,7 +1511,7 @@
       <c r="L47" s="8"/>
       <c r="M47" s="8"/>
     </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
@@ -1502,7 +1525,7 @@
       <c r="L48" s="8"/>
       <c r="M48" s="8"/>
     </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
@@ -1516,7 +1539,7 @@
       <c r="L49" s="8"/>
       <c r="M49" s="8"/>
     </row>
-    <row r="50" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
@@ -1530,7 +1553,7 @@
       <c r="L50" s="8"/>
       <c r="M50" s="8"/>
     </row>
-    <row r="51" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
@@ -1544,7 +1567,7 @@
       <c r="L51" s="8"/>
       <c r="M51" s="8"/>
     </row>
-    <row r="52" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
@@ -1558,7 +1581,7 @@
       <c r="L52" s="8"/>
       <c r="M52" s="8"/>
     </row>
-    <row r="53" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
@@ -1572,7 +1595,7 @@
       <c r="L53" s="8"/>
       <c r="M53" s="8"/>
     </row>
-    <row r="54" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
@@ -1586,7 +1609,7 @@
       <c r="L54" s="8"/>
       <c r="M54" s="8"/>
     </row>
-    <row r="55" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
@@ -1600,7 +1623,7 @@
       <c r="L55" s="8"/>
       <c r="M55" s="8"/>
     </row>
-    <row r="56" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
@@ -1614,7 +1637,7 @@
       <c r="L56" s="8"/>
       <c r="M56" s="8"/>
     </row>
-    <row r="57" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
@@ -1628,7 +1651,7 @@
       <c r="L57" s="8"/>
       <c r="M57" s="8"/>
     </row>
-    <row r="58" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
@@ -1642,7 +1665,7 @@
       <c r="L58" s="8"/>
       <c r="M58" s="8"/>
     </row>
-    <row r="59" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
       <c r="D59" s="5"/>
@@ -1656,7 +1679,7 @@
       <c r="L59" s="8"/>
       <c r="M59" s="8"/>
     </row>
-    <row r="60" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
@@ -1670,7 +1693,7 @@
       <c r="L60" s="8"/>
       <c r="M60" s="8"/>
     </row>
-    <row r="61" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
@@ -1684,7 +1707,7 @@
       <c r="L61" s="8"/>
       <c r="M61" s="8"/>
     </row>
-    <row r="62" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
@@ -1698,7 +1721,7 @@
       <c r="L62" s="8"/>
       <c r="M62" s="8"/>
     </row>
-    <row r="63" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
@@ -1712,7 +1735,7 @@
       <c r="L63" s="8"/>
       <c r="M63" s="8"/>
     </row>
-    <row r="64" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
@@ -1726,7 +1749,7 @@
       <c r="L64" s="8"/>
       <c r="M64" s="8"/>
     </row>
-    <row r="65" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B65" s="5"/>
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
@@ -1740,7 +1763,7 @@
       <c r="L65" s="8"/>
       <c r="M65" s="8"/>
     </row>
-    <row r="66" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
@@ -1754,7 +1777,7 @@
       <c r="L66" s="8"/>
       <c r="M66" s="8"/>
     </row>
-    <row r="67" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
       <c r="D67" s="5"/>
@@ -1768,7 +1791,7 @@
       <c r="L67" s="8"/>
       <c r="M67" s="8"/>
     </row>
-    <row r="68" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
@@ -1782,7 +1805,7 @@
       <c r="L68" s="8"/>
       <c r="M68" s="8"/>
     </row>
-    <row r="69" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B69" s="5"/>
       <c r="C69" s="5"/>
       <c r="D69" s="5"/>
@@ -1796,7 +1819,7 @@
       <c r="L69" s="8"/>
       <c r="M69" s="8"/>
     </row>
-    <row r="70" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B70" s="5"/>
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
@@ -1810,7 +1833,7 @@
       <c r="L70" s="8"/>
       <c r="M70" s="8"/>
     </row>
-    <row r="71" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B71" s="5"/>
       <c r="C71" s="5"/>
       <c r="D71" s="5"/>
@@ -1824,7 +1847,7 @@
       <c r="L71" s="8"/>
       <c r="M71" s="8"/>
     </row>
-    <row r="72" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
@@ -1838,7 +1861,7 @@
       <c r="L72" s="8"/>
       <c r="M72" s="8"/>
     </row>
-    <row r="73" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B73" s="5"/>
       <c r="C73" s="5"/>
       <c r="D73" s="5"/>
@@ -1852,7 +1875,7 @@
       <c r="L73" s="8"/>
       <c r="M73" s="8"/>
     </row>
-    <row r="74" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B74" s="5"/>
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
@@ -1866,7 +1889,7 @@
       <c r="L74" s="8"/>
       <c r="M74" s="8"/>
     </row>
-    <row r="75" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B75" s="5"/>
       <c r="C75" s="5"/>
       <c r="D75" s="5"/>
@@ -1880,7 +1903,7 @@
       <c r="L75" s="8"/>
       <c r="M75" s="8"/>
     </row>
-    <row r="76" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B76" s="5"/>
       <c r="C76" s="5"/>
       <c r="D76" s="5"/>
@@ -1894,7 +1917,7 @@
       <c r="L76" s="8"/>
       <c r="M76" s="8"/>
     </row>
-    <row r="77" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B77" s="5"/>
       <c r="C77" s="5"/>
       <c r="D77" s="5"/>
@@ -1908,7 +1931,7 @@
       <c r="L77" s="8"/>
       <c r="M77" s="8"/>
     </row>
-    <row r="78" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B78" s="5"/>
       <c r="C78" s="5"/>
       <c r="D78" s="5"/>
@@ -1922,7 +1945,7 @@
       <c r="L78" s="8"/>
       <c r="M78" s="8"/>
     </row>
-    <row r="79" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B79" s="5"/>
       <c r="C79" s="5"/>
       <c r="D79" s="5"/>
@@ -1936,7 +1959,7 @@
       <c r="L79" s="8"/>
       <c r="M79" s="8"/>
     </row>
-    <row r="80" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B80" s="5"/>
       <c r="C80" s="5"/>
       <c r="D80" s="5"/>
@@ -1950,7 +1973,7 @@
       <c r="L80" s="8"/>
       <c r="M80" s="8"/>
     </row>
-    <row r="81" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B81" s="5"/>
       <c r="C81" s="5"/>
       <c r="D81" s="5"/>
@@ -1964,7 +1987,7 @@
       <c r="L81" s="8"/>
       <c r="M81" s="8"/>
     </row>
-    <row r="82" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B82" s="5"/>
       <c r="C82" s="5"/>
       <c r="D82" s="5"/>
@@ -1978,7 +2001,7 @@
       <c r="L82" s="8"/>
       <c r="M82" s="8"/>
     </row>
-    <row r="83" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B83" s="5"/>
       <c r="C83" s="5"/>
       <c r="D83" s="5"/>
@@ -1992,7 +2015,7 @@
       <c r="L83" s="8"/>
       <c r="M83" s="8"/>
     </row>
-    <row r="84" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B84" s="5"/>
       <c r="C84" s="5"/>
       <c r="D84" s="5"/>
@@ -2006,7 +2029,7 @@
       <c r="L84" s="8"/>
       <c r="M84" s="8"/>
     </row>
-    <row r="85" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B85" s="5"/>
       <c r="C85" s="5"/>
       <c r="D85" s="5"/>
@@ -2020,7 +2043,7 @@
       <c r="L85" s="8"/>
       <c r="M85" s="8"/>
     </row>
-    <row r="86" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
       <c r="D86" s="5"/>
@@ -2034,7 +2057,7 @@
       <c r="L86" s="8"/>
       <c r="M86" s="8"/>
     </row>
-    <row r="87" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B87" s="5"/>
       <c r="C87" s="5"/>
       <c r="D87" s="5"/>
@@ -2048,7 +2071,7 @@
       <c r="L87" s="8"/>
       <c r="M87" s="8"/>
     </row>
-    <row r="88" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B88" s="5"/>
       <c r="C88" s="5"/>
       <c r="D88" s="5"/>
@@ -2062,7 +2085,7 @@
       <c r="L88" s="8"/>
       <c r="M88" s="8"/>
     </row>
-    <row r="89" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B89" s="5"/>
       <c r="C89" s="5"/>
       <c r="D89" s="5"/>
@@ -2076,7 +2099,7 @@
       <c r="L89" s="8"/>
       <c r="M89" s="8"/>
     </row>
-    <row r="90" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B90" s="5"/>
       <c r="C90" s="5"/>
       <c r="D90" s="5"/>
@@ -2090,7 +2113,7 @@
       <c r="L90" s="8"/>
       <c r="M90" s="8"/>
     </row>
-    <row r="91" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B91" s="5"/>
       <c r="C91" s="5"/>
       <c r="D91" s="5"/>
@@ -2104,7 +2127,7 @@
       <c r="L91" s="8"/>
       <c r="M91" s="8"/>
     </row>
-    <row r="92" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B92" s="5"/>
       <c r="C92" s="5"/>
       <c r="D92" s="5"/>
@@ -2118,7 +2141,7 @@
       <c r="L92" s="8"/>
       <c r="M92" s="8"/>
     </row>
-    <row r="93" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B93" s="5"/>
       <c r="C93" s="5"/>
       <c r="D93" s="5"/>
@@ -2132,7 +2155,7 @@
       <c r="L93" s="8"/>
       <c r="M93" s="8"/>
     </row>
-    <row r="94" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B94" s="5"/>
       <c r="C94" s="5"/>
       <c r="D94" s="5"/>
@@ -2146,7 +2169,7 @@
       <c r="L94" s="8"/>
       <c r="M94" s="8"/>
     </row>
-    <row r="95" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B95" s="5"/>
       <c r="C95" s="5"/>
       <c r="D95" s="5"/>
@@ -2160,7 +2183,7 @@
       <c r="L95" s="8"/>
       <c r="M95" s="8"/>
     </row>
-    <row r="96" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B96" s="5"/>
       <c r="C96" s="5"/>
       <c r="D96" s="5"/>
@@ -2174,7 +2197,7 @@
       <c r="L96" s="8"/>
       <c r="M96" s="8"/>
     </row>
-    <row r="97" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B97" s="5"/>
       <c r="C97" s="5"/>
       <c r="D97" s="5"/>
@@ -2188,7 +2211,7 @@
       <c r="L97" s="8"/>
       <c r="M97" s="8"/>
     </row>
-    <row r="98" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B98" s="5"/>
       <c r="C98" s="5"/>
       <c r="D98" s="5"/>
@@ -2202,7 +2225,7 @@
       <c r="L98" s="8"/>
       <c r="M98" s="8"/>
     </row>
-    <row r="99" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B99" s="5"/>
       <c r="C99" s="5"/>
       <c r="D99" s="5"/>
@@ -2216,7 +2239,7 @@
       <c r="L99" s="8"/>
       <c r="M99" s="8"/>
     </row>
-    <row r="100" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B100" s="5"/>
       <c r="C100" s="5"/>
       <c r="D100" s="5"/>
@@ -2230,7 +2253,7 @@
       <c r="L100" s="8"/>
       <c r="M100" s="8"/>
     </row>
-    <row r="101" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B101" s="5"/>
       <c r="C101" s="5"/>
       <c r="D101" s="5"/>
@@ -2244,7 +2267,7 @@
       <c r="L101" s="8"/>
       <c r="M101" s="8"/>
     </row>
-    <row r="102" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B102" s="5"/>
       <c r="C102" s="5"/>
       <c r="D102" s="5"/>
@@ -2258,7 +2281,7 @@
       <c r="L102" s="8"/>
       <c r="M102" s="8"/>
     </row>
-    <row r="103" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B103" s="5"/>
       <c r="C103" s="5"/>
       <c r="D103" s="5"/>
@@ -2272,7 +2295,7 @@
       <c r="L103" s="8"/>
       <c r="M103" s="8"/>
     </row>
-    <row r="104" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B104" s="5"/>
       <c r="C104" s="5"/>
       <c r="D104" s="5"/>
@@ -2286,7 +2309,7 @@
       <c r="L104" s="8"/>
       <c r="M104" s="8"/>
     </row>
-    <row r="105" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B105" s="5"/>
       <c r="C105" s="5"/>
       <c r="D105" s="5"/>
@@ -2300,7 +2323,7 @@
       <c r="L105" s="8"/>
       <c r="M105" s="8"/>
     </row>
-    <row r="106" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B106" s="5"/>
       <c r="C106" s="5"/>
       <c r="D106" s="5"/>
@@ -2314,7 +2337,7 @@
       <c r="L106" s="8"/>
       <c r="M106" s="8"/>
     </row>
-    <row r="107" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B107" s="5"/>
       <c r="C107" s="5"/>
       <c r="D107" s="5"/>
@@ -2328,7 +2351,7 @@
       <c r="L107" s="8"/>
       <c r="M107" s="8"/>
     </row>
-    <row r="108" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B108" s="5"/>
       <c r="C108" s="5"/>
       <c r="D108" s="5"/>
@@ -2342,7 +2365,7 @@
       <c r="L108" s="8"/>
       <c r="M108" s="8"/>
     </row>
-    <row r="109" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B109" s="5"/>
       <c r="C109" s="5"/>
       <c r="D109" s="5"/>
@@ -2356,7 +2379,7 @@
       <c r="L109" s="8"/>
       <c r="M109" s="8"/>
     </row>
-    <row r="110" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B110" s="5"/>
       <c r="C110" s="5"/>
       <c r="D110" s="5"/>
@@ -2370,7 +2393,7 @@
       <c r="L110" s="8"/>
       <c r="M110" s="8"/>
     </row>
-    <row r="111" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B111" s="5"/>
       <c r="C111" s="5"/>
       <c r="D111" s="5"/>
@@ -2384,7 +2407,7 @@
       <c r="L111" s="8"/>
       <c r="M111" s="8"/>
     </row>
-    <row r="112" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B112" s="5"/>
       <c r="C112" s="5"/>
       <c r="D112" s="5"/>
@@ -2398,7 +2421,7 @@
       <c r="L112" s="8"/>
       <c r="M112" s="8"/>
     </row>
-    <row r="113" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B113" s="5"/>
       <c r="C113" s="5"/>
       <c r="D113" s="5"/>
@@ -2412,7 +2435,7 @@
       <c r="L113" s="8"/>
       <c r="M113" s="8"/>
     </row>
-    <row r="114" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B114" s="5"/>
       <c r="C114" s="5"/>
       <c r="D114" s="5"/>
@@ -2426,7 +2449,7 @@
       <c r="L114" s="8"/>
       <c r="M114" s="8"/>
     </row>
-    <row r="115" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B115" s="5"/>
       <c r="C115" s="5"/>
       <c r="D115" s="5"/>
@@ -2440,7 +2463,7 @@
       <c r="L115" s="8"/>
       <c r="M115" s="8"/>
     </row>
-    <row r="116" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B116" s="5"/>
       <c r="C116" s="5"/>
       <c r="D116" s="5"/>
@@ -2454,7 +2477,7 @@
       <c r="L116" s="8"/>
       <c r="M116" s="8"/>
     </row>
-    <row r="117" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="117" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B117" s="5"/>
       <c r="C117" s="5"/>
       <c r="D117" s="5"/>
@@ -2468,7 +2491,7 @@
       <c r="L117" s="8"/>
       <c r="M117" s="8"/>
     </row>
-    <row r="118" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="118" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B118" s="5"/>
       <c r="C118" s="5"/>
       <c r="D118" s="5"/>
@@ -2482,7 +2505,7 @@
       <c r="L118" s="8"/>
       <c r="M118" s="8"/>
     </row>
-    <row r="119" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="119" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B119" s="5"/>
       <c r="C119" s="5"/>
       <c r="D119" s="5"/>
@@ -2496,7 +2519,7 @@
       <c r="L119" s="8"/>
       <c r="M119" s="8"/>
     </row>
-    <row r="120" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="120" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B120" s="5"/>
       <c r="C120" s="5"/>
       <c r="D120" s="5"/>
@@ -2510,7 +2533,7 @@
       <c r="L120" s="8"/>
       <c r="M120" s="8"/>
     </row>
-    <row r="121" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="121" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B121" s="5"/>
       <c r="C121" s="5"/>
       <c r="D121" s="5"/>
@@ -2524,7 +2547,7 @@
       <c r="L121" s="8"/>
       <c r="M121" s="8"/>
     </row>
-    <row r="122" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B122" s="5"/>
       <c r="C122" s="5"/>
       <c r="D122" s="5"/>
@@ -2538,7 +2561,7 @@
       <c r="L122" s="8"/>
       <c r="M122" s="8"/>
     </row>
-    <row r="123" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="123" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B123" s="5"/>
       <c r="C123" s="5"/>
       <c r="D123" s="5"/>
@@ -2552,7 +2575,7 @@
       <c r="L123" s="8"/>
       <c r="M123" s="8"/>
     </row>
-    <row r="124" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="124" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B124" s="5"/>
       <c r="C124" s="5"/>
       <c r="D124" s="5"/>
@@ -2566,7 +2589,7 @@
       <c r="L124" s="8"/>
       <c r="M124" s="8"/>
     </row>
-    <row r="125" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="125" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B125" s="5"/>
       <c r="C125" s="5"/>
       <c r="D125" s="5"/>
@@ -2580,7 +2603,7 @@
       <c r="L125" s="8"/>
       <c r="M125" s="8"/>
     </row>
-    <row r="126" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="126" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B126" s="5"/>
       <c r="C126" s="5"/>
       <c r="D126" s="5"/>
@@ -2594,7 +2617,7 @@
       <c r="L126" s="8"/>
       <c r="M126" s="8"/>
     </row>
-    <row r="127" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="127" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B127" s="5"/>
       <c r="C127" s="5"/>
       <c r="D127" s="5"/>
@@ -2608,7 +2631,7 @@
       <c r="L127" s="8"/>
       <c r="M127" s="8"/>
     </row>
-    <row r="128" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="128" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B128" s="5"/>
       <c r="C128" s="5"/>
       <c r="D128" s="5"/>
@@ -2622,7 +2645,7 @@
       <c r="L128" s="8"/>
       <c r="M128" s="8"/>
     </row>
-    <row r="129" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="129" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B129" s="5"/>
       <c r="C129" s="5"/>
       <c r="D129" s="5"/>
@@ -2636,7 +2659,7 @@
       <c r="L129" s="8"/>
       <c r="M129" s="8"/>
     </row>
-    <row r="130" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="130" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B130" s="5"/>
       <c r="C130" s="5"/>
       <c r="D130" s="5"/>
@@ -2650,7 +2673,7 @@
       <c r="L130" s="8"/>
       <c r="M130" s="8"/>
     </row>
-    <row r="131" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="131" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B131" s="5"/>
       <c r="C131" s="5"/>
       <c r="D131" s="5"/>
@@ -2664,7 +2687,7 @@
       <c r="L131" s="8"/>
       <c r="M131" s="8"/>
     </row>
-    <row r="132" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="132" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B132" s="5"/>
       <c r="C132" s="5"/>
       <c r="D132" s="5"/>
@@ -2678,7 +2701,7 @@
       <c r="L132" s="8"/>
       <c r="M132" s="8"/>
     </row>
-    <row r="133" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="133" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B133" s="5"/>
       <c r="C133" s="5"/>
       <c r="D133" s="5"/>
@@ -2692,7 +2715,7 @@
       <c r="L133" s="8"/>
       <c r="M133" s="8"/>
     </row>
-    <row r="134" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="134" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B134" s="5"/>
       <c r="C134" s="5"/>
       <c r="D134" s="5"/>
@@ -2706,7 +2729,7 @@
       <c r="L134" s="8"/>
       <c r="M134" s="8"/>
     </row>
-    <row r="135" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="135" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B135" s="5"/>
       <c r="C135" s="5"/>
       <c r="D135" s="5"/>
@@ -2720,7 +2743,7 @@
       <c r="L135" s="8"/>
       <c r="M135" s="8"/>
     </row>
-    <row r="136" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="136" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B136" s="5"/>
       <c r="C136" s="5"/>
       <c r="D136" s="5"/>
@@ -2734,7 +2757,7 @@
       <c r="L136" s="8"/>
       <c r="M136" s="8"/>
     </row>
-    <row r="137" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="137" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B137" s="5"/>
       <c r="C137" s="5"/>
       <c r="D137" s="5"/>
@@ -2748,7 +2771,7 @@
       <c r="L137" s="8"/>
       <c r="M137" s="8"/>
     </row>
-    <row r="138" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="138" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B138" s="5"/>
       <c r="C138" s="5"/>
       <c r="D138" s="5"/>
@@ -2762,7 +2785,7 @@
       <c r="L138" s="8"/>
       <c r="M138" s="8"/>
     </row>
-    <row r="139" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="139" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B139" s="5"/>
       <c r="C139" s="5"/>
       <c r="D139" s="5"/>
@@ -2776,7 +2799,7 @@
       <c r="L139" s="8"/>
       <c r="M139" s="8"/>
     </row>
-    <row r="140" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="140" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B140" s="5"/>
       <c r="C140" s="5"/>
       <c r="D140" s="5"/>
@@ -2790,7 +2813,7 @@
       <c r="L140" s="8"/>
       <c r="M140" s="8"/>
     </row>
-    <row r="141" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="141" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B141" s="5"/>
       <c r="C141" s="5"/>
       <c r="D141" s="5"/>
@@ -2804,7 +2827,7 @@
       <c r="L141" s="8"/>
       <c r="M141" s="8"/>
     </row>
-    <row r="142" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="142" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B142" s="5"/>
       <c r="C142" s="5"/>
       <c r="D142" s="5"/>
@@ -2818,7 +2841,7 @@
       <c r="L142" s="8"/>
       <c r="M142" s="8"/>
     </row>
-    <row r="143" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="143" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B143" s="5"/>
       <c r="C143" s="5"/>
       <c r="D143" s="5"/>
@@ -2832,7 +2855,7 @@
       <c r="L143" s="8"/>
       <c r="M143" s="8"/>
     </row>
-    <row r="144" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="144" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B144" s="5"/>
       <c r="C144" s="5"/>
       <c r="D144" s="5"/>
@@ -2846,7 +2869,7 @@
       <c r="L144" s="8"/>
       <c r="M144" s="8"/>
     </row>
-    <row r="145" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="145" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B145" s="5"/>
       <c r="C145" s="5"/>
       <c r="D145" s="5"/>
@@ -2860,7 +2883,7 @@
       <c r="L145" s="8"/>
       <c r="M145" s="8"/>
     </row>
-    <row r="146" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="146" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B146" s="5"/>
       <c r="C146" s="5"/>
       <c r="D146" s="5"/>
@@ -2874,7 +2897,7 @@
       <c r="L146" s="8"/>
       <c r="M146" s="8"/>
     </row>
-    <row r="147" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="147" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B147" s="5"/>
       <c r="C147" s="5"/>
       <c r="D147" s="5"/>
@@ -2888,7 +2911,7 @@
       <c r="L147" s="8"/>
       <c r="M147" s="8"/>
     </row>
-    <row r="148" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="148" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B148" s="5"/>
       <c r="C148" s="5"/>
       <c r="D148" s="5"/>
@@ -2902,7 +2925,7 @@
       <c r="L148" s="8"/>
       <c r="M148" s="8"/>
     </row>
-    <row r="149" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="149" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B149" s="5"/>
       <c r="C149" s="5"/>
       <c r="D149" s="5"/>
@@ -2916,7 +2939,7 @@
       <c r="L149" s="8"/>
       <c r="M149" s="8"/>
     </row>
-    <row r="150" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="150" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B150" s="5"/>
       <c r="C150" s="5"/>
       <c r="D150" s="5"/>
@@ -2930,7 +2953,7 @@
       <c r="L150" s="8"/>
       <c r="M150" s="8"/>
     </row>
-    <row r="151" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="151" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B151" s="5"/>
       <c r="C151" s="5"/>
       <c r="D151" s="5"/>
@@ -2944,7 +2967,7 @@
       <c r="L151" s="8"/>
       <c r="M151" s="8"/>
     </row>
-    <row r="152" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="152" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B152" s="5"/>
       <c r="C152" s="5"/>
       <c r="D152" s="5"/>
@@ -2958,7 +2981,7 @@
       <c r="L152" s="8"/>
       <c r="M152" s="8"/>
     </row>
-    <row r="153" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="153" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B153" s="5"/>
       <c r="C153" s="5"/>
       <c r="D153" s="5"/>
@@ -2972,7 +2995,7 @@
       <c r="L153" s="8"/>
       <c r="M153" s="8"/>
     </row>
-    <row r="154" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="154" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B154" s="5"/>
       <c r="C154" s="5"/>
       <c r="D154" s="5"/>
@@ -2986,7 +3009,7 @@
       <c r="L154" s="8"/>
       <c r="M154" s="8"/>
     </row>
-    <row r="155" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="155" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B155" s="5"/>
       <c r="C155" s="5"/>
       <c r="D155" s="5"/>
@@ -3000,7 +3023,7 @@
       <c r="L155" s="8"/>
       <c r="M155" s="8"/>
     </row>
-    <row r="156" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="156" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B156" s="5"/>
       <c r="C156" s="5"/>
       <c r="D156" s="5"/>
@@ -3014,7 +3037,7 @@
       <c r="L156" s="8"/>
       <c r="M156" s="8"/>
     </row>
-    <row r="157" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="157" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B157" s="5"/>
       <c r="C157" s="5"/>
       <c r="D157" s="5"/>
@@ -3028,7 +3051,7 @@
       <c r="L157" s="8"/>
       <c r="M157" s="8"/>
     </row>
-    <row r="158" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="158" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B158" s="5"/>
       <c r="C158" s="5"/>
       <c r="D158" s="5"/>
@@ -3042,7 +3065,7 @@
       <c r="L158" s="8"/>
       <c r="M158" s="8"/>
     </row>
-    <row r="159" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="159" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B159" s="5"/>
       <c r="C159" s="5"/>
       <c r="D159" s="5"/>
@@ -3056,7 +3079,7 @@
       <c r="L159" s="8"/>
       <c r="M159" s="8"/>
     </row>
-    <row r="160" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="160" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B160" s="5"/>
       <c r="C160" s="5"/>
       <c r="D160" s="5"/>
@@ -3070,7 +3093,7 @@
       <c r="L160" s="8"/>
       <c r="M160" s="8"/>
     </row>
-    <row r="161" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="161" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B161" s="5"/>
       <c r="C161" s="5"/>
       <c r="D161" s="5"/>
@@ -3084,7 +3107,7 @@
       <c r="L161" s="8"/>
       <c r="M161" s="8"/>
     </row>
-    <row r="162" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="162" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B162" s="5"/>
       <c r="C162" s="5"/>
       <c r="D162" s="5"/>
@@ -3098,7 +3121,7 @@
       <c r="L162" s="8"/>
       <c r="M162" s="8"/>
     </row>
-    <row r="163" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="163" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B163" s="5"/>
       <c r="C163" s="5"/>
       <c r="D163" s="5"/>
@@ -3112,7 +3135,7 @@
       <c r="L163" s="8"/>
       <c r="M163" s="8"/>
     </row>
-    <row r="164" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="164" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B164" s="5"/>
       <c r="C164" s="5"/>
       <c r="D164" s="5"/>
@@ -3126,7 +3149,7 @@
       <c r="L164" s="8"/>
       <c r="M164" s="8"/>
     </row>
-    <row r="165" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="165" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B165" s="5"/>
       <c r="C165" s="5"/>
       <c r="D165" s="5"/>
@@ -3140,7 +3163,7 @@
       <c r="L165" s="8"/>
       <c r="M165" s="8"/>
     </row>
-    <row r="166" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="166" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B166" s="5"/>
       <c r="C166" s="5"/>
       <c r="D166" s="5"/>
@@ -3154,7 +3177,7 @@
       <c r="L166" s="8"/>
       <c r="M166" s="8"/>
     </row>
-    <row r="167" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="167" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B167" s="5"/>
       <c r="C167" s="5"/>
       <c r="D167" s="5"/>
@@ -3168,7 +3191,7 @@
       <c r="L167" s="8"/>
       <c r="M167" s="8"/>
     </row>
-    <row r="168" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="168" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B168" s="5"/>
       <c r="C168" s="5"/>
       <c r="D168" s="5"/>
@@ -3182,7 +3205,7 @@
       <c r="L168" s="8"/>
       <c r="M168" s="8"/>
     </row>
-    <row r="169" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="169" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B169" s="5"/>
       <c r="C169" s="5"/>
       <c r="D169" s="5"/>
@@ -3196,7 +3219,7 @@
       <c r="L169" s="8"/>
       <c r="M169" s="8"/>
     </row>
-    <row r="170" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="170" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B170" s="5"/>
       <c r="C170" s="5"/>
       <c r="D170" s="5"/>
@@ -3210,7 +3233,7 @@
       <c r="L170" s="8"/>
       <c r="M170" s="8"/>
     </row>
-    <row r="171" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="171" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B171" s="5"/>
       <c r="C171" s="5"/>
       <c r="D171" s="5"/>
@@ -3224,7 +3247,7 @@
       <c r="L171" s="8"/>
       <c r="M171" s="8"/>
     </row>
-    <row r="172" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="172" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B172" s="5"/>
       <c r="C172" s="5"/>
       <c r="D172" s="5"/>
@@ -3238,7 +3261,7 @@
       <c r="L172" s="8"/>
       <c r="M172" s="8"/>
     </row>
-    <row r="173" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="173" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B173" s="5"/>
       <c r="C173" s="5"/>
       <c r="D173" s="5"/>
@@ -3252,7 +3275,7 @@
       <c r="L173" s="8"/>
       <c r="M173" s="8"/>
     </row>
-    <row r="174" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="174" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B174" s="5"/>
       <c r="C174" s="5"/>
       <c r="D174" s="5"/>
@@ -3266,7 +3289,7 @@
       <c r="L174" s="8"/>
       <c r="M174" s="8"/>
     </row>
-    <row r="175" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="175" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B175" s="5"/>
       <c r="C175" s="5"/>
       <c r="D175" s="5"/>
@@ -3280,7 +3303,7 @@
       <c r="L175" s="8"/>
       <c r="M175" s="8"/>
     </row>
-    <row r="176" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="176" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B176" s="5"/>
       <c r="C176" s="5"/>
       <c r="D176" s="5"/>
@@ -3294,7 +3317,7 @@
       <c r="L176" s="8"/>
       <c r="M176" s="8"/>
     </row>
-    <row r="177" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="177" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B177" s="5"/>
       <c r="C177" s="5"/>
       <c r="D177" s="5"/>
@@ -3308,7 +3331,7 @@
       <c r="L177" s="8"/>
       <c r="M177" s="8"/>
     </row>
-    <row r="178" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="178" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B178" s="5"/>
       <c r="C178" s="5"/>
       <c r="D178" s="5"/>
@@ -3322,7 +3345,7 @@
       <c r="L178" s="8"/>
       <c r="M178" s="8"/>
     </row>
-    <row r="179" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="179" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B179" s="5"/>
       <c r="C179" s="5"/>
       <c r="D179" s="5"/>
@@ -3336,7 +3359,7 @@
       <c r="L179" s="8"/>
       <c r="M179" s="8"/>
     </row>
-    <row r="180" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="180" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B180" s="5"/>
       <c r="C180" s="5"/>
       <c r="D180" s="5"/>
@@ -3350,7 +3373,7 @@
       <c r="L180" s="8"/>
       <c r="M180" s="8"/>
     </row>
-    <row r="181" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="181" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B181" s="5"/>
       <c r="C181" s="5"/>
       <c r="D181" s="5"/>
@@ -3364,7 +3387,7 @@
       <c r="L181" s="8"/>
       <c r="M181" s="8"/>
     </row>
-    <row r="182" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="182" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B182" s="5"/>
       <c r="C182" s="5"/>
       <c r="D182" s="5"/>
@@ -3378,7 +3401,7 @@
       <c r="L182" s="8"/>
       <c r="M182" s="8"/>
     </row>
-    <row r="183" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="183" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B183" s="5"/>
       <c r="C183" s="5"/>
       <c r="D183" s="5"/>
@@ -3392,7 +3415,7 @@
       <c r="L183" s="8"/>
       <c r="M183" s="8"/>
     </row>
-    <row r="184" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="184" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B184" s="5"/>
       <c r="C184" s="5"/>
       <c r="D184" s="5"/>
@@ -3406,7 +3429,7 @@
       <c r="L184" s="8"/>
       <c r="M184" s="8"/>
     </row>
-    <row r="185" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="185" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B185" s="5"/>
       <c r="C185" s="5"/>
       <c r="D185" s="5"/>
@@ -3420,7 +3443,7 @@
       <c r="L185" s="8"/>
       <c r="M185" s="8"/>
     </row>
-    <row r="186" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="186" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B186" s="5"/>
       <c r="C186" s="5"/>
       <c r="D186" s="5"/>
@@ -3434,7 +3457,7 @@
       <c r="L186" s="8"/>
       <c r="M186" s="8"/>
     </row>
-    <row r="187" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="187" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B187" s="5"/>
       <c r="C187" s="5"/>
       <c r="D187" s="5"/>
@@ -3448,7 +3471,7 @@
       <c r="L187" s="8"/>
       <c r="M187" s="8"/>
     </row>
-    <row r="188" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="188" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B188" s="5"/>
       <c r="C188" s="5"/>
       <c r="D188" s="5"/>
@@ -3462,7 +3485,7 @@
       <c r="L188" s="8"/>
       <c r="M188" s="8"/>
     </row>
-    <row r="189" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="189" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B189" s="5"/>
       <c r="C189" s="5"/>
       <c r="D189" s="5"/>
@@ -3476,7 +3499,7 @@
       <c r="L189" s="8"/>
       <c r="M189" s="8"/>
     </row>
-    <row r="190" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="190" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B190" s="5"/>
       <c r="C190" s="5"/>
       <c r="D190" s="5"/>
@@ -3490,7 +3513,7 @@
       <c r="L190" s="8"/>
       <c r="M190" s="8"/>
     </row>
-    <row r="191" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="191" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B191" s="5"/>
       <c r="C191" s="5"/>
       <c r="D191" s="5"/>
@@ -3504,7 +3527,7 @@
       <c r="L191" s="8"/>
       <c r="M191" s="8"/>
     </row>
-    <row r="192" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="192" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B192" s="5"/>
       <c r="C192" s="5"/>
       <c r="D192" s="5"/>
@@ -3518,7 +3541,7 @@
       <c r="L192" s="8"/>
       <c r="M192" s="8"/>
     </row>
-    <row r="193" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="193" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B193" s="5"/>
       <c r="C193" s="5"/>
       <c r="D193" s="5"/>
@@ -3532,7 +3555,7 @@
       <c r="L193" s="8"/>
       <c r="M193" s="8"/>
     </row>
-    <row r="194" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="194" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B194" s="5"/>
       <c r="C194" s="5"/>
       <c r="D194" s="5"/>
@@ -3546,7 +3569,7 @@
       <c r="L194" s="8"/>
       <c r="M194" s="8"/>
     </row>
-    <row r="195" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="195" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B195" s="5"/>
       <c r="C195" s="5"/>
       <c r="D195" s="5"/>
@@ -3560,7 +3583,7 @@
       <c r="L195" s="8"/>
       <c r="M195" s="8"/>
     </row>
-    <row r="196" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="196" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B196" s="5"/>
       <c r="C196" s="5"/>
       <c r="D196" s="5"/>
@@ -3574,7 +3597,7 @@
       <c r="L196" s="8"/>
       <c r="M196" s="8"/>
     </row>
-    <row r="197" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="197" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B197" s="5"/>
       <c r="C197" s="5"/>
       <c r="D197" s="5"/>
@@ -3588,7 +3611,7 @@
       <c r="L197" s="8"/>
       <c r="M197" s="8"/>
     </row>
-    <row r="198" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="198" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B198" s="5"/>
       <c r="C198" s="5"/>
       <c r="D198" s="5"/>
@@ -3602,7 +3625,7 @@
       <c r="L198" s="8"/>
       <c r="M198" s="8"/>
     </row>
-    <row r="199" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="199" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B199" s="5"/>
       <c r="C199" s="5"/>
       <c r="D199" s="5"/>
@@ -3616,7 +3639,7 @@
       <c r="L199" s="8"/>
       <c r="M199" s="8"/>
     </row>
-    <row r="200" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="200" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B200" s="5"/>
       <c r="C200" s="5"/>
       <c r="D200" s="5"/>
@@ -3632,8 +3655,8 @@
     </row>
   </sheetData>
   <autoFilter ref="B4:N4" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:N9">
-      <sortCondition descending="1" ref="H4:H9"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:N10">
+      <sortCondition descending="1" ref="H4"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3646,20 +3669,20 @@
   <dimension ref="A2:J200"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:K8"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.5" customWidth="1"/>
-    <col min="2" max="9" width="14.6640625" customWidth="1"/>
-    <col min="10" max="10" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="2.453125" customWidth="1"/>
+    <col min="2" max="9" width="14.6328125" customWidth="1"/>
+    <col min="10" max="10" width="15.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="13" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
@@ -3667,34 +3690,34 @@
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
       <c r="H2" s="16" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="I2" s="19">
-        <v>44902</v>
+        <v>44903</v>
       </c>
       <c r="J2" s="19"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B3" s="10" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="18"/>
       <c r="F3" s="12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B4" s="10" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D4" s="20"/>
       <c r="E4" s="21"/>
       <c r="F4" s="11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B6" s="4" t="s">
         <v>1</v>
       </c>
@@ -3705,51 +3728,51 @@
         <v>3</v>
       </c>
       <c r="E6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="4" t="s">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B7" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>27</v>
-      </c>
       <c r="E7" s="5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F7" s="7">
-        <v>2.2999999999999998</v>
+        <v>1.7</v>
       </c>
       <c r="G7" s="9">
-        <v>22000</v>
+        <v>200000</v>
       </c>
       <c r="H7" s="9">
         <f>F7*G7</f>
-        <v>50599.999999999993</v>
+        <v>340000</v>
       </c>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -3760,7 +3783,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -3771,7 +3794,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -3782,7 +3805,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -3792,7 +3815,7 @@
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -3802,7 +3825,7 @@
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -3812,7 +3835,7 @@
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -3822,7 +3845,7 @@
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -3832,7 +3855,7 @@
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -3842,7 +3865,7 @@
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -3852,7 +3875,7 @@
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -3862,7 +3885,7 @@
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -3872,7 +3895,7 @@
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
@@ -3882,7 +3905,7 @@
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
@@ -3892,7 +3915,7 @@
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
@@ -3902,7 +3925,7 @@
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -3912,7 +3935,7 @@
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -3922,7 +3945,7 @@
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
@@ -3932,7 +3955,7 @@
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
@@ -3942,7 +3965,7 @@
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
@@ -3952,7 +3975,7 @@
       <c r="H27" s="6"/>
       <c r="I27" s="6"/>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
@@ -3962,7 +3985,7 @@
       <c r="H28" s="6"/>
       <c r="I28" s="6"/>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
@@ -3972,7 +3995,7 @@
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
@@ -3982,7 +4005,7 @@
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
@@ -3992,7 +4015,7 @@
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -4002,7 +4025,7 @@
       <c r="H32" s="6"/>
       <c r="I32" s="6"/>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
@@ -4012,7 +4035,7 @@
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -4022,7 +4045,7 @@
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
@@ -4032,7 +4055,7 @@
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
@@ -4042,7 +4065,7 @@
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
@@ -4052,7 +4075,7 @@
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
@@ -4062,7 +4085,7 @@
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
@@ -4072,7 +4095,7 @@
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
@@ -4082,7 +4105,7 @@
       <c r="H40" s="6"/>
       <c r="I40" s="6"/>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
@@ -4092,7 +4115,7 @@
       <c r="H41" s="6"/>
       <c r="I41" s="6"/>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
@@ -4102,7 +4125,7 @@
       <c r="H42" s="6"/>
       <c r="I42" s="6"/>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
@@ -4112,7 +4135,7 @@
       <c r="H43" s="6"/>
       <c r="I43" s="6"/>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
@@ -4122,7 +4145,7 @@
       <c r="H44" s="6"/>
       <c r="I44" s="6"/>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
@@ -4132,7 +4155,7 @@
       <c r="H45" s="6"/>
       <c r="I45" s="6"/>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
@@ -4142,7 +4165,7 @@
       <c r="H46" s="6"/>
       <c r="I46" s="6"/>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
@@ -4152,7 +4175,7 @@
       <c r="H47" s="6"/>
       <c r="I47" s="6"/>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
@@ -4162,7 +4185,7 @@
       <c r="H48" s="6"/>
       <c r="I48" s="6"/>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
@@ -4172,7 +4195,7 @@
       <c r="H49" s="6"/>
       <c r="I49" s="6"/>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
@@ -4182,7 +4205,7 @@
       <c r="H50" s="6"/>
       <c r="I50" s="6"/>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
@@ -4192,7 +4215,7 @@
       <c r="H51" s="6"/>
       <c r="I51" s="6"/>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
@@ -4202,7 +4225,7 @@
       <c r="H52" s="6"/>
       <c r="I52" s="6"/>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
@@ -4212,7 +4235,7 @@
       <c r="H53" s="6"/>
       <c r="I53" s="6"/>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
@@ -4222,7 +4245,7 @@
       <c r="H54" s="6"/>
       <c r="I54" s="6"/>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
@@ -4232,7 +4255,7 @@
       <c r="H55" s="6"/>
       <c r="I55" s="6"/>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
@@ -4242,7 +4265,7 @@
       <c r="H56" s="6"/>
       <c r="I56" s="6"/>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
@@ -4252,7 +4275,7 @@
       <c r="H57" s="6"/>
       <c r="I57" s="6"/>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
@@ -4262,7 +4285,7 @@
       <c r="H58" s="6"/>
       <c r="I58" s="6"/>
     </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
       <c r="D59" s="5"/>
@@ -4272,7 +4295,7 @@
       <c r="H59" s="6"/>
       <c r="I59" s="6"/>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
@@ -4282,7 +4305,7 @@
       <c r="H60" s="6"/>
       <c r="I60" s="6"/>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
@@ -4292,7 +4315,7 @@
       <c r="H61" s="6"/>
       <c r="I61" s="6"/>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
@@ -4302,7 +4325,7 @@
       <c r="H62" s="6"/>
       <c r="I62" s="6"/>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
@@ -4312,7 +4335,7 @@
       <c r="H63" s="6"/>
       <c r="I63" s="6"/>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
@@ -4322,7 +4345,7 @@
       <c r="H64" s="6"/>
       <c r="I64" s="6"/>
     </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B65" s="5"/>
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
@@ -4332,7 +4355,7 @@
       <c r="H65" s="6"/>
       <c r="I65" s="6"/>
     </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
@@ -4342,7 +4365,7 @@
       <c r="H66" s="6"/>
       <c r="I66" s="6"/>
     </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
       <c r="D67" s="5"/>
@@ -4352,7 +4375,7 @@
       <c r="H67" s="6"/>
       <c r="I67" s="6"/>
     </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
@@ -4362,7 +4385,7 @@
       <c r="H68" s="6"/>
       <c r="I68" s="6"/>
     </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B69" s="5"/>
       <c r="C69" s="5"/>
       <c r="D69" s="5"/>
@@ -4372,7 +4395,7 @@
       <c r="H69" s="6"/>
       <c r="I69" s="6"/>
     </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B70" s="5"/>
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
@@ -4382,7 +4405,7 @@
       <c r="H70" s="6"/>
       <c r="I70" s="6"/>
     </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B71" s="5"/>
       <c r="C71" s="5"/>
       <c r="D71" s="5"/>
@@ -4392,7 +4415,7 @@
       <c r="H71" s="6"/>
       <c r="I71" s="6"/>
     </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
@@ -4402,7 +4425,7 @@
       <c r="H72" s="6"/>
       <c r="I72" s="6"/>
     </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B73" s="5"/>
       <c r="C73" s="5"/>
       <c r="D73" s="5"/>
@@ -4412,7 +4435,7 @@
       <c r="H73" s="6"/>
       <c r="I73" s="6"/>
     </row>
-    <row r="74" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B74" s="5"/>
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
@@ -4422,7 +4445,7 @@
       <c r="H74" s="6"/>
       <c r="I74" s="6"/>
     </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B75" s="5"/>
       <c r="C75" s="5"/>
       <c r="D75" s="5"/>
@@ -4432,7 +4455,7 @@
       <c r="H75" s="6"/>
       <c r="I75" s="6"/>
     </row>
-    <row r="76" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B76" s="5"/>
       <c r="C76" s="5"/>
       <c r="D76" s="5"/>
@@ -4442,7 +4465,7 @@
       <c r="H76" s="6"/>
       <c r="I76" s="6"/>
     </row>
-    <row r="77" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B77" s="5"/>
       <c r="C77" s="5"/>
       <c r="D77" s="5"/>
@@ -4452,7 +4475,7 @@
       <c r="H77" s="6"/>
       <c r="I77" s="6"/>
     </row>
-    <row r="78" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B78" s="5"/>
       <c r="C78" s="5"/>
       <c r="D78" s="5"/>
@@ -4462,7 +4485,7 @@
       <c r="H78" s="6"/>
       <c r="I78" s="6"/>
     </row>
-    <row r="79" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B79" s="5"/>
       <c r="C79" s="5"/>
       <c r="D79" s="5"/>
@@ -4472,7 +4495,7 @@
       <c r="H79" s="6"/>
       <c r="I79" s="6"/>
     </row>
-    <row r="80" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B80" s="5"/>
       <c r="C80" s="5"/>
       <c r="D80" s="5"/>
@@ -4482,7 +4505,7 @@
       <c r="H80" s="6"/>
       <c r="I80" s="6"/>
     </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B81" s="5"/>
       <c r="C81" s="5"/>
       <c r="D81" s="5"/>
@@ -4492,7 +4515,7 @@
       <c r="H81" s="6"/>
       <c r="I81" s="6"/>
     </row>
-    <row r="82" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B82" s="5"/>
       <c r="C82" s="5"/>
       <c r="D82" s="5"/>
@@ -4502,7 +4525,7 @@
       <c r="H82" s="6"/>
       <c r="I82" s="6"/>
     </row>
-    <row r="83" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B83" s="5"/>
       <c r="C83" s="5"/>
       <c r="D83" s="5"/>
@@ -4512,7 +4535,7 @@
       <c r="H83" s="6"/>
       <c r="I83" s="6"/>
     </row>
-    <row r="84" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B84" s="5"/>
       <c r="C84" s="5"/>
       <c r="D84" s="5"/>
@@ -4522,7 +4545,7 @@
       <c r="H84" s="6"/>
       <c r="I84" s="6"/>
     </row>
-    <row r="85" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B85" s="5"/>
       <c r="C85" s="5"/>
       <c r="D85" s="5"/>
@@ -4532,7 +4555,7 @@
       <c r="H85" s="6"/>
       <c r="I85" s="6"/>
     </row>
-    <row r="86" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
       <c r="D86" s="5"/>
@@ -4542,7 +4565,7 @@
       <c r="H86" s="6"/>
       <c r="I86" s="6"/>
     </row>
-    <row r="87" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B87" s="5"/>
       <c r="C87" s="5"/>
       <c r="D87" s="5"/>
@@ -4552,7 +4575,7 @@
       <c r="H87" s="6"/>
       <c r="I87" s="6"/>
     </row>
-    <row r="88" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B88" s="5"/>
       <c r="C88" s="5"/>
       <c r="D88" s="5"/>
@@ -4562,7 +4585,7 @@
       <c r="H88" s="6"/>
       <c r="I88" s="6"/>
     </row>
-    <row r="89" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B89" s="5"/>
       <c r="C89" s="5"/>
       <c r="D89" s="5"/>
@@ -4572,7 +4595,7 @@
       <c r="H89" s="6"/>
       <c r="I89" s="6"/>
     </row>
-    <row r="90" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B90" s="5"/>
       <c r="C90" s="5"/>
       <c r="D90" s="5"/>
@@ -4582,7 +4605,7 @@
       <c r="H90" s="6"/>
       <c r="I90" s="6"/>
     </row>
-    <row r="91" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B91" s="5"/>
       <c r="C91" s="5"/>
       <c r="D91" s="5"/>
@@ -4592,7 +4615,7 @@
       <c r="H91" s="6"/>
       <c r="I91" s="6"/>
     </row>
-    <row r="92" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B92" s="5"/>
       <c r="C92" s="5"/>
       <c r="D92" s="5"/>
@@ -4602,7 +4625,7 @@
       <c r="H92" s="6"/>
       <c r="I92" s="6"/>
     </row>
-    <row r="93" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B93" s="5"/>
       <c r="C93" s="5"/>
       <c r="D93" s="5"/>
@@ -4612,7 +4635,7 @@
       <c r="H93" s="6"/>
       <c r="I93" s="6"/>
     </row>
-    <row r="94" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B94" s="5"/>
       <c r="C94" s="5"/>
       <c r="D94" s="5"/>
@@ -4622,7 +4645,7 @@
       <c r="H94" s="6"/>
       <c r="I94" s="6"/>
     </row>
-    <row r="95" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B95" s="5"/>
       <c r="C95" s="5"/>
       <c r="D95" s="5"/>
@@ -4632,7 +4655,7 @@
       <c r="H95" s="6"/>
       <c r="I95" s="6"/>
     </row>
-    <row r="96" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B96" s="5"/>
       <c r="C96" s="5"/>
       <c r="D96" s="5"/>
@@ -4642,7 +4665,7 @@
       <c r="H96" s="6"/>
       <c r="I96" s="6"/>
     </row>
-    <row r="97" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B97" s="5"/>
       <c r="C97" s="5"/>
       <c r="D97" s="5"/>
@@ -4652,7 +4675,7 @@
       <c r="H97" s="6"/>
       <c r="I97" s="6"/>
     </row>
-    <row r="98" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B98" s="5"/>
       <c r="C98" s="5"/>
       <c r="D98" s="5"/>
@@ -4662,7 +4685,7 @@
       <c r="H98" s="6"/>
       <c r="I98" s="6"/>
     </row>
-    <row r="99" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B99" s="5"/>
       <c r="C99" s="5"/>
       <c r="D99" s="5"/>
@@ -4672,7 +4695,7 @@
       <c r="H99" s="6"/>
       <c r="I99" s="6"/>
     </row>
-    <row r="100" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B100" s="5"/>
       <c r="C100" s="5"/>
       <c r="D100" s="5"/>
@@ -4682,7 +4705,7 @@
       <c r="H100" s="6"/>
       <c r="I100" s="6"/>
     </row>
-    <row r="101" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B101" s="5"/>
       <c r="C101" s="5"/>
       <c r="D101" s="5"/>
@@ -4692,7 +4715,7 @@
       <c r="H101" s="6"/>
       <c r="I101" s="6"/>
     </row>
-    <row r="102" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B102" s="5"/>
       <c r="C102" s="5"/>
       <c r="D102" s="5"/>
@@ -4702,7 +4725,7 @@
       <c r="H102" s="6"/>
       <c r="I102" s="6"/>
     </row>
-    <row r="103" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B103" s="5"/>
       <c r="C103" s="5"/>
       <c r="D103" s="5"/>
@@ -4712,7 +4735,7 @@
       <c r="H103" s="6"/>
       <c r="I103" s="6"/>
     </row>
-    <row r="104" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B104" s="5"/>
       <c r="C104" s="5"/>
       <c r="D104" s="5"/>
@@ -4722,7 +4745,7 @@
       <c r="H104" s="6"/>
       <c r="I104" s="6"/>
     </row>
-    <row r="105" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B105" s="5"/>
       <c r="C105" s="5"/>
       <c r="D105" s="5"/>
@@ -4732,7 +4755,7 @@
       <c r="H105" s="6"/>
       <c r="I105" s="6"/>
     </row>
-    <row r="106" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B106" s="5"/>
       <c r="C106" s="5"/>
       <c r="D106" s="5"/>
@@ -4742,7 +4765,7 @@
       <c r="H106" s="6"/>
       <c r="I106" s="6"/>
     </row>
-    <row r="107" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B107" s="5"/>
       <c r="C107" s="5"/>
       <c r="D107" s="5"/>
@@ -4752,7 +4775,7 @@
       <c r="H107" s="6"/>
       <c r="I107" s="6"/>
     </row>
-    <row r="108" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B108" s="5"/>
       <c r="C108" s="5"/>
       <c r="D108" s="5"/>
@@ -4762,7 +4785,7 @@
       <c r="H108" s="6"/>
       <c r="I108" s="6"/>
     </row>
-    <row r="109" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B109" s="5"/>
       <c r="C109" s="5"/>
       <c r="D109" s="5"/>
@@ -4772,7 +4795,7 @@
       <c r="H109" s="6"/>
       <c r="I109" s="6"/>
     </row>
-    <row r="110" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B110" s="5"/>
       <c r="C110" s="5"/>
       <c r="D110" s="5"/>
@@ -4782,7 +4805,7 @@
       <c r="H110" s="6"/>
       <c r="I110" s="6"/>
     </row>
-    <row r="111" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B111" s="5"/>
       <c r="C111" s="5"/>
       <c r="D111" s="5"/>
@@ -4792,7 +4815,7 @@
       <c r="H111" s="6"/>
       <c r="I111" s="6"/>
     </row>
-    <row r="112" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B112" s="5"/>
       <c r="C112" s="5"/>
       <c r="D112" s="5"/>
@@ -4802,7 +4825,7 @@
       <c r="H112" s="6"/>
       <c r="I112" s="6"/>
     </row>
-    <row r="113" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B113" s="5"/>
       <c r="C113" s="5"/>
       <c r="D113" s="5"/>
@@ -4812,7 +4835,7 @@
       <c r="H113" s="6"/>
       <c r="I113" s="6"/>
     </row>
-    <row r="114" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B114" s="5"/>
       <c r="C114" s="5"/>
       <c r="D114" s="5"/>
@@ -4822,7 +4845,7 @@
       <c r="H114" s="6"/>
       <c r="I114" s="6"/>
     </row>
-    <row r="115" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B115" s="5"/>
       <c r="C115" s="5"/>
       <c r="D115" s="5"/>
@@ -4832,7 +4855,7 @@
       <c r="H115" s="6"/>
       <c r="I115" s="6"/>
     </row>
-    <row r="116" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B116" s="5"/>
       <c r="C116" s="5"/>
       <c r="D116" s="5"/>
@@ -4842,7 +4865,7 @@
       <c r="H116" s="6"/>
       <c r="I116" s="6"/>
     </row>
-    <row r="117" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="117" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B117" s="5"/>
       <c r="C117" s="5"/>
       <c r="D117" s="5"/>
@@ -4852,7 +4875,7 @@
       <c r="H117" s="6"/>
       <c r="I117" s="6"/>
     </row>
-    <row r="118" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="118" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B118" s="5"/>
       <c r="C118" s="5"/>
       <c r="D118" s="5"/>
@@ -4862,7 +4885,7 @@
       <c r="H118" s="6"/>
       <c r="I118" s="6"/>
     </row>
-    <row r="119" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="119" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B119" s="5"/>
       <c r="C119" s="5"/>
       <c r="D119" s="5"/>
@@ -4872,7 +4895,7 @@
       <c r="H119" s="6"/>
       <c r="I119" s="6"/>
     </row>
-    <row r="120" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="120" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B120" s="5"/>
       <c r="C120" s="5"/>
       <c r="D120" s="5"/>
@@ -4882,7 +4905,7 @@
       <c r="H120" s="6"/>
       <c r="I120" s="6"/>
     </row>
-    <row r="121" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="121" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B121" s="5"/>
       <c r="C121" s="5"/>
       <c r="D121" s="5"/>
@@ -4892,7 +4915,7 @@
       <c r="H121" s="6"/>
       <c r="I121" s="6"/>
     </row>
-    <row r="122" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B122" s="5"/>
       <c r="C122" s="5"/>
       <c r="D122" s="5"/>
@@ -4902,7 +4925,7 @@
       <c r="H122" s="6"/>
       <c r="I122" s="6"/>
     </row>
-    <row r="123" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="123" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B123" s="5"/>
       <c r="C123" s="5"/>
       <c r="D123" s="5"/>
@@ -4912,7 +4935,7 @@
       <c r="H123" s="6"/>
       <c r="I123" s="6"/>
     </row>
-    <row r="124" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="124" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B124" s="5"/>
       <c r="C124" s="5"/>
       <c r="D124" s="5"/>
@@ -4922,7 +4945,7 @@
       <c r="H124" s="6"/>
       <c r="I124" s="6"/>
     </row>
-    <row r="125" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="125" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B125" s="5"/>
       <c r="C125" s="5"/>
       <c r="D125" s="5"/>
@@ -4932,7 +4955,7 @@
       <c r="H125" s="6"/>
       <c r="I125" s="6"/>
     </row>
-    <row r="126" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="126" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B126" s="5"/>
       <c r="C126" s="5"/>
       <c r="D126" s="5"/>
@@ -4942,7 +4965,7 @@
       <c r="H126" s="6"/>
       <c r="I126" s="6"/>
     </row>
-    <row r="127" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="127" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B127" s="5"/>
       <c r="C127" s="5"/>
       <c r="D127" s="5"/>
@@ -4952,7 +4975,7 @@
       <c r="H127" s="6"/>
       <c r="I127" s="6"/>
     </row>
-    <row r="128" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="128" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B128" s="5"/>
       <c r="C128" s="5"/>
       <c r="D128" s="5"/>
@@ -4962,7 +4985,7 @@
       <c r="H128" s="6"/>
       <c r="I128" s="6"/>
     </row>
-    <row r="129" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="129" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B129" s="5"/>
       <c r="C129" s="5"/>
       <c r="D129" s="5"/>
@@ -4972,7 +4995,7 @@
       <c r="H129" s="6"/>
       <c r="I129" s="6"/>
     </row>
-    <row r="130" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="130" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B130" s="5"/>
       <c r="C130" s="5"/>
       <c r="D130" s="5"/>
@@ -4982,7 +5005,7 @@
       <c r="H130" s="6"/>
       <c r="I130" s="6"/>
     </row>
-    <row r="131" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="131" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B131" s="5"/>
       <c r="C131" s="5"/>
       <c r="D131" s="5"/>
@@ -4992,7 +5015,7 @@
       <c r="H131" s="6"/>
       <c r="I131" s="6"/>
     </row>
-    <row r="132" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="132" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B132" s="5"/>
       <c r="C132" s="5"/>
       <c r="D132" s="5"/>
@@ -5002,7 +5025,7 @@
       <c r="H132" s="6"/>
       <c r="I132" s="6"/>
     </row>
-    <row r="133" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="133" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B133" s="5"/>
       <c r="C133" s="5"/>
       <c r="D133" s="5"/>
@@ -5012,7 +5035,7 @@
       <c r="H133" s="6"/>
       <c r="I133" s="6"/>
     </row>
-    <row r="134" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="134" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B134" s="5"/>
       <c r="C134" s="5"/>
       <c r="D134" s="5"/>
@@ -5022,7 +5045,7 @@
       <c r="H134" s="6"/>
       <c r="I134" s="6"/>
     </row>
-    <row r="135" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="135" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B135" s="5"/>
       <c r="C135" s="5"/>
       <c r="D135" s="5"/>
@@ -5032,7 +5055,7 @@
       <c r="H135" s="6"/>
       <c r="I135" s="6"/>
     </row>
-    <row r="136" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="136" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B136" s="5"/>
       <c r="C136" s="5"/>
       <c r="D136" s="5"/>
@@ -5042,7 +5065,7 @@
       <c r="H136" s="6"/>
       <c r="I136" s="6"/>
     </row>
-    <row r="137" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="137" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B137" s="5"/>
       <c r="C137" s="5"/>
       <c r="D137" s="5"/>
@@ -5052,7 +5075,7 @@
       <c r="H137" s="6"/>
       <c r="I137" s="6"/>
     </row>
-    <row r="138" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="138" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B138" s="5"/>
       <c r="C138" s="5"/>
       <c r="D138" s="5"/>
@@ -5062,7 +5085,7 @@
       <c r="H138" s="6"/>
       <c r="I138" s="6"/>
     </row>
-    <row r="139" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="139" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B139" s="5"/>
       <c r="C139" s="5"/>
       <c r="D139" s="5"/>
@@ -5072,7 +5095,7 @@
       <c r="H139" s="6"/>
       <c r="I139" s="6"/>
     </row>
-    <row r="140" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="140" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B140" s="5"/>
       <c r="C140" s="5"/>
       <c r="D140" s="5"/>
@@ -5082,7 +5105,7 @@
       <c r="H140" s="6"/>
       <c r="I140" s="6"/>
     </row>
-    <row r="141" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="141" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B141" s="5"/>
       <c r="C141" s="5"/>
       <c r="D141" s="5"/>
@@ -5092,7 +5115,7 @@
       <c r="H141" s="6"/>
       <c r="I141" s="6"/>
     </row>
-    <row r="142" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="142" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B142" s="5"/>
       <c r="C142" s="5"/>
       <c r="D142" s="5"/>
@@ -5102,7 +5125,7 @@
       <c r="H142" s="6"/>
       <c r="I142" s="6"/>
     </row>
-    <row r="143" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="143" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B143" s="5"/>
       <c r="C143" s="5"/>
       <c r="D143" s="5"/>
@@ -5112,7 +5135,7 @@
       <c r="H143" s="6"/>
       <c r="I143" s="6"/>
     </row>
-    <row r="144" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="144" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B144" s="5"/>
       <c r="C144" s="5"/>
       <c r="D144" s="5"/>
@@ -5122,7 +5145,7 @@
       <c r="H144" s="6"/>
       <c r="I144" s="6"/>
     </row>
-    <row r="145" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="145" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B145" s="5"/>
       <c r="C145" s="5"/>
       <c r="D145" s="5"/>
@@ -5132,7 +5155,7 @@
       <c r="H145" s="6"/>
       <c r="I145" s="6"/>
     </row>
-    <row r="146" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="146" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B146" s="5"/>
       <c r="C146" s="5"/>
       <c r="D146" s="5"/>
@@ -5142,7 +5165,7 @@
       <c r="H146" s="6"/>
       <c r="I146" s="6"/>
     </row>
-    <row r="147" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="147" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B147" s="5"/>
       <c r="C147" s="5"/>
       <c r="D147" s="5"/>
@@ -5152,7 +5175,7 @@
       <c r="H147" s="6"/>
       <c r="I147" s="6"/>
     </row>
-    <row r="148" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="148" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B148" s="5"/>
       <c r="C148" s="5"/>
       <c r="D148" s="5"/>
@@ -5162,7 +5185,7 @@
       <c r="H148" s="6"/>
       <c r="I148" s="6"/>
     </row>
-    <row r="149" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="149" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B149" s="5"/>
       <c r="C149" s="5"/>
       <c r="D149" s="5"/>
@@ -5172,7 +5195,7 @@
       <c r="H149" s="6"/>
       <c r="I149" s="6"/>
     </row>
-    <row r="150" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="150" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B150" s="5"/>
       <c r="C150" s="5"/>
       <c r="D150" s="5"/>
@@ -5182,7 +5205,7 @@
       <c r="H150" s="6"/>
       <c r="I150" s="6"/>
     </row>
-    <row r="151" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="151" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B151" s="5"/>
       <c r="C151" s="5"/>
       <c r="D151" s="5"/>
@@ -5192,7 +5215,7 @@
       <c r="H151" s="6"/>
       <c r="I151" s="6"/>
     </row>
-    <row r="152" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="152" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B152" s="5"/>
       <c r="C152" s="5"/>
       <c r="D152" s="5"/>
@@ -5202,7 +5225,7 @@
       <c r="H152" s="6"/>
       <c r="I152" s="6"/>
     </row>
-    <row r="153" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="153" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B153" s="5"/>
       <c r="C153" s="5"/>
       <c r="D153" s="5"/>
@@ -5212,7 +5235,7 @@
       <c r="H153" s="6"/>
       <c r="I153" s="6"/>
     </row>
-    <row r="154" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="154" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B154" s="5"/>
       <c r="C154" s="5"/>
       <c r="D154" s="5"/>
@@ -5222,7 +5245,7 @@
       <c r="H154" s="6"/>
       <c r="I154" s="6"/>
     </row>
-    <row r="155" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="155" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B155" s="5"/>
       <c r="C155" s="5"/>
       <c r="D155" s="5"/>
@@ -5232,7 +5255,7 @@
       <c r="H155" s="6"/>
       <c r="I155" s="6"/>
     </row>
-    <row r="156" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="156" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B156" s="5"/>
       <c r="C156" s="5"/>
       <c r="D156" s="5"/>
@@ -5242,7 +5265,7 @@
       <c r="H156" s="6"/>
       <c r="I156" s="6"/>
     </row>
-    <row r="157" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="157" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B157" s="5"/>
       <c r="C157" s="5"/>
       <c r="D157" s="5"/>
@@ -5252,7 +5275,7 @@
       <c r="H157" s="6"/>
       <c r="I157" s="6"/>
     </row>
-    <row r="158" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="158" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B158" s="5"/>
       <c r="C158" s="5"/>
       <c r="D158" s="5"/>
@@ -5262,7 +5285,7 @@
       <c r="H158" s="6"/>
       <c r="I158" s="6"/>
     </row>
-    <row r="159" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="159" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B159" s="5"/>
       <c r="C159" s="5"/>
       <c r="D159" s="5"/>
@@ -5272,7 +5295,7 @@
       <c r="H159" s="6"/>
       <c r="I159" s="6"/>
     </row>
-    <row r="160" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="160" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B160" s="5"/>
       <c r="C160" s="5"/>
       <c r="D160" s="5"/>
@@ -5282,7 +5305,7 @@
       <c r="H160" s="6"/>
       <c r="I160" s="6"/>
     </row>
-    <row r="161" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="161" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B161" s="5"/>
       <c r="C161" s="5"/>
       <c r="D161" s="5"/>
@@ -5292,7 +5315,7 @@
       <c r="H161" s="6"/>
       <c r="I161" s="6"/>
     </row>
-    <row r="162" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="162" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B162" s="5"/>
       <c r="C162" s="5"/>
       <c r="D162" s="5"/>
@@ -5302,7 +5325,7 @@
       <c r="H162" s="6"/>
       <c r="I162" s="6"/>
     </row>
-    <row r="163" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="163" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B163" s="5"/>
       <c r="C163" s="5"/>
       <c r="D163" s="5"/>
@@ -5312,7 +5335,7 @@
       <c r="H163" s="6"/>
       <c r="I163" s="6"/>
     </row>
-    <row r="164" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="164" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B164" s="5"/>
       <c r="C164" s="5"/>
       <c r="D164" s="5"/>
@@ -5322,7 +5345,7 @@
       <c r="H164" s="6"/>
       <c r="I164" s="6"/>
     </row>
-    <row r="165" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="165" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B165" s="5"/>
       <c r="C165" s="5"/>
       <c r="D165" s="5"/>
@@ -5332,7 +5355,7 @@
       <c r="H165" s="6"/>
       <c r="I165" s="6"/>
     </row>
-    <row r="166" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="166" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B166" s="5"/>
       <c r="C166" s="5"/>
       <c r="D166" s="5"/>
@@ -5342,7 +5365,7 @@
       <c r="H166" s="6"/>
       <c r="I166" s="6"/>
     </row>
-    <row r="167" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="167" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B167" s="5"/>
       <c r="C167" s="5"/>
       <c r="D167" s="5"/>
@@ -5352,7 +5375,7 @@
       <c r="H167" s="6"/>
       <c r="I167" s="6"/>
     </row>
-    <row r="168" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="168" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B168" s="5"/>
       <c r="C168" s="5"/>
       <c r="D168" s="5"/>
@@ -5362,7 +5385,7 @@
       <c r="H168" s="6"/>
       <c r="I168" s="6"/>
     </row>
-    <row r="169" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="169" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B169" s="5"/>
       <c r="C169" s="5"/>
       <c r="D169" s="5"/>
@@ -5372,7 +5395,7 @@
       <c r="H169" s="6"/>
       <c r="I169" s="6"/>
     </row>
-    <row r="170" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="170" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B170" s="5"/>
       <c r="C170" s="5"/>
       <c r="D170" s="5"/>
@@ -5382,7 +5405,7 @@
       <c r="H170" s="6"/>
       <c r="I170" s="6"/>
     </row>
-    <row r="171" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="171" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B171" s="5"/>
       <c r="C171" s="5"/>
       <c r="D171" s="5"/>
@@ -5392,7 +5415,7 @@
       <c r="H171" s="6"/>
       <c r="I171" s="6"/>
     </row>
-    <row r="172" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="172" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B172" s="5"/>
       <c r="C172" s="5"/>
       <c r="D172" s="5"/>
@@ -5402,7 +5425,7 @@
       <c r="H172" s="6"/>
       <c r="I172" s="6"/>
     </row>
-    <row r="173" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="173" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B173" s="5"/>
       <c r="C173" s="5"/>
       <c r="D173" s="5"/>
@@ -5412,7 +5435,7 @@
       <c r="H173" s="6"/>
       <c r="I173" s="6"/>
     </row>
-    <row r="174" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="174" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B174" s="5"/>
       <c r="C174" s="5"/>
       <c r="D174" s="5"/>
@@ -5422,7 +5445,7 @@
       <c r="H174" s="6"/>
       <c r="I174" s="6"/>
     </row>
-    <row r="175" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="175" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B175" s="5"/>
       <c r="C175" s="5"/>
       <c r="D175" s="5"/>
@@ -5432,7 +5455,7 @@
       <c r="H175" s="6"/>
       <c r="I175" s="6"/>
     </row>
-    <row r="176" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="176" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B176" s="5"/>
       <c r="C176" s="5"/>
       <c r="D176" s="5"/>
@@ -5442,7 +5465,7 @@
       <c r="H176" s="6"/>
       <c r="I176" s="6"/>
     </row>
-    <row r="177" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="177" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B177" s="5"/>
       <c r="C177" s="5"/>
       <c r="D177" s="5"/>
@@ -5452,7 +5475,7 @@
       <c r="H177" s="6"/>
       <c r="I177" s="6"/>
     </row>
-    <row r="178" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="178" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B178" s="5"/>
       <c r="C178" s="5"/>
       <c r="D178" s="5"/>
@@ -5462,7 +5485,7 @@
       <c r="H178" s="6"/>
       <c r="I178" s="6"/>
     </row>
-    <row r="179" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="179" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B179" s="5"/>
       <c r="C179" s="5"/>
       <c r="D179" s="5"/>
@@ -5472,7 +5495,7 @@
       <c r="H179" s="6"/>
       <c r="I179" s="6"/>
     </row>
-    <row r="180" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="180" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B180" s="5"/>
       <c r="C180" s="5"/>
       <c r="D180" s="5"/>
@@ -5482,7 +5505,7 @@
       <c r="H180" s="6"/>
       <c r="I180" s="6"/>
     </row>
-    <row r="181" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="181" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B181" s="5"/>
       <c r="C181" s="5"/>
       <c r="D181" s="5"/>
@@ -5492,7 +5515,7 @@
       <c r="H181" s="6"/>
       <c r="I181" s="6"/>
     </row>
-    <row r="182" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="182" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B182" s="5"/>
       <c r="C182" s="5"/>
       <c r="D182" s="5"/>
@@ -5502,7 +5525,7 @@
       <c r="H182" s="6"/>
       <c r="I182" s="6"/>
     </row>
-    <row r="183" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="183" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B183" s="5"/>
       <c r="C183" s="5"/>
       <c r="D183" s="5"/>
@@ -5512,7 +5535,7 @@
       <c r="H183" s="6"/>
       <c r="I183" s="6"/>
     </row>
-    <row r="184" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="184" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B184" s="5"/>
       <c r="C184" s="5"/>
       <c r="D184" s="5"/>
@@ -5522,7 +5545,7 @@
       <c r="H184" s="6"/>
       <c r="I184" s="6"/>
     </row>
-    <row r="185" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="185" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B185" s="5"/>
       <c r="C185" s="5"/>
       <c r="D185" s="5"/>
@@ -5532,7 +5555,7 @@
       <c r="H185" s="6"/>
       <c r="I185" s="6"/>
     </row>
-    <row r="186" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="186" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B186" s="5"/>
       <c r="C186" s="5"/>
       <c r="D186" s="5"/>
@@ -5542,7 +5565,7 @@
       <c r="H186" s="6"/>
       <c r="I186" s="6"/>
     </row>
-    <row r="187" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="187" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B187" s="5"/>
       <c r="C187" s="5"/>
       <c r="D187" s="5"/>
@@ -5552,7 +5575,7 @@
       <c r="H187" s="6"/>
       <c r="I187" s="6"/>
     </row>
-    <row r="188" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="188" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B188" s="5"/>
       <c r="C188" s="5"/>
       <c r="D188" s="5"/>
@@ -5562,7 +5585,7 @@
       <c r="H188" s="6"/>
       <c r="I188" s="6"/>
     </row>
-    <row r="189" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="189" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B189" s="5"/>
       <c r="C189" s="5"/>
       <c r="D189" s="5"/>
@@ -5572,7 +5595,7 @@
       <c r="H189" s="6"/>
       <c r="I189" s="6"/>
     </row>
-    <row r="190" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="190" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B190" s="5"/>
       <c r="C190" s="5"/>
       <c r="D190" s="5"/>
@@ -5582,7 +5605,7 @@
       <c r="H190" s="6"/>
       <c r="I190" s="6"/>
     </row>
-    <row r="191" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="191" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B191" s="5"/>
       <c r="C191" s="5"/>
       <c r="D191" s="5"/>
@@ -5592,7 +5615,7 @@
       <c r="H191" s="6"/>
       <c r="I191" s="6"/>
     </row>
-    <row r="192" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="192" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B192" s="5"/>
       <c r="C192" s="5"/>
       <c r="D192" s="5"/>
@@ -5602,7 +5625,7 @@
       <c r="H192" s="6"/>
       <c r="I192" s="6"/>
     </row>
-    <row r="193" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="193" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B193" s="5"/>
       <c r="C193" s="5"/>
       <c r="D193" s="5"/>
@@ -5612,7 +5635,7 @@
       <c r="H193" s="6"/>
       <c r="I193" s="6"/>
     </row>
-    <row r="194" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="194" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B194" s="5"/>
       <c r="C194" s="5"/>
       <c r="D194" s="5"/>
@@ -5622,7 +5645,7 @@
       <c r="H194" s="6"/>
       <c r="I194" s="6"/>
     </row>
-    <row r="195" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="195" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B195" s="5"/>
       <c r="C195" s="5"/>
       <c r="D195" s="5"/>
@@ -5632,7 +5655,7 @@
       <c r="H195" s="6"/>
       <c r="I195" s="6"/>
     </row>
-    <row r="196" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="196" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B196" s="5"/>
       <c r="C196" s="5"/>
       <c r="D196" s="5"/>
@@ -5642,7 +5665,7 @@
       <c r="H196" s="6"/>
       <c r="I196" s="6"/>
     </row>
-    <row r="197" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="197" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B197" s="5"/>
       <c r="C197" s="5"/>
       <c r="D197" s="5"/>
@@ -5652,7 +5675,7 @@
       <c r="H197" s="6"/>
       <c r="I197" s="6"/>
     </row>
-    <row r="198" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="198" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B198" s="5"/>
       <c r="C198" s="5"/>
       <c r="D198" s="5"/>
@@ -5662,7 +5685,7 @@
       <c r="H198" s="6"/>
       <c r="I198" s="6"/>
     </row>
-    <row r="199" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="199" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B199" s="5"/>
       <c r="C199" s="5"/>
       <c r="D199" s="5"/>
@@ -5672,7 +5695,7 @@
       <c r="H199" s="6"/>
       <c r="I199" s="6"/>
     </row>
-    <row r="200" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="200" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B200" s="5"/>
       <c r="C200" s="5"/>
       <c r="D200" s="5"/>

</xml_diff>

<commit_message>
fixed a bug with the figures_in
</commit_message>
<xml_diff>
--- a/Opportunities/Pipeline_monitor/Pipeline_monitor.xlsx
+++ b/Opportunities/Pipeline_monitor/Pipeline_monitor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jerry.chen\PycharmProjects\pythonProject\Opportunities\Pipeline_monitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6376DB72-894F-48C3-844D-4149708F18F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{55D61EFF-B55B-4DCE-8FB4-147E40269BCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1900" yWindow="1900" windowWidth="14400" windowHeight="7360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Monitor" sheetId="1" r:id="rId1"/>
@@ -73,15 +73,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>0806.HK</t>
-  </si>
-  <si>
-    <t>VALUE PARTNERS</t>
-  </si>
-  <si>
-    <t>HKG</t>
-  </si>
-  <si>
     <t>Current Holdings Monitor</t>
   </si>
   <si>
@@ -121,16 +112,25 @@
     <t xml:space="preserve">Total Protfolio at FV = </t>
   </si>
   <si>
+    <t>0697.HK</t>
+  </si>
+  <si>
+    <t>SHOUCHENG</t>
+  </si>
+  <si>
+    <t>HKG</t>
+  </si>
+  <si>
+    <t>0806.HK</t>
+  </si>
+  <si>
+    <t>VALUE PARTNERS</t>
+  </si>
+  <si>
     <t>1475.HK</t>
   </si>
   <si>
     <t>NISSIN FOODS</t>
-  </si>
-  <si>
-    <t>0697.HK</t>
-  </si>
-  <si>
-    <t>SHOUCHENG</t>
   </si>
   <si>
     <t>3718.HK</t>
@@ -684,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:N200"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -738,7 +738,7 @@
         <v>7</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>8</v>
@@ -750,7 +750,7 @@
         <v>10</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>11</v>
@@ -758,36 +758,36 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B5" s="5" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="E5" s="7">
-        <v>0.67</v>
+        <v>1.73</v>
       </c>
       <c r="F5" s="6">
-        <v>0.1720746953370591</v>
+        <v>0.11290796645794088</v>
       </c>
       <c r="G5" s="6">
-        <v>0.11018690726749793</v>
+        <v>9.7865360759977885E-2</v>
       </c>
       <c r="H5" s="6">
         <f>F5-G5</f>
-        <v>6.1887788069561175E-2</v>
+        <v>1.5042605697962994E-2</v>
       </c>
       <c r="I5" s="5">
-        <v>7.0000000000000007E-2</v>
+        <v>9.6099999999999991E-2</v>
       </c>
       <c r="J5" s="6">
         <f>I5/E5</f>
-        <v>0.10447761194029852</v>
+        <v>5.5549132947976872E-2</v>
       </c>
       <c r="K5" s="7">
-        <v>0.48</v>
+        <v>1.35</v>
       </c>
       <c r="L5" s="8">
         <v>44925</v>
@@ -798,40 +798,42 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B6" s="5" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="E6" s="7">
-        <v>23880000</v>
+        <v>2.65</v>
       </c>
       <c r="F6" s="6">
-        <v>6.4027111830930822E-2</v>
+        <v>4.427808325428817E-2</v>
       </c>
       <c r="G6" s="6">
-        <v>5.6776003015075377E-2</v>
+        <v>9.3811838619443283E-2</v>
       </c>
       <c r="H6" s="6">
         <f>F6-G6</f>
-        <v>7.2511088158554449E-3</v>
+        <v>-4.9533755365155113E-2</v>
       </c>
       <c r="I6" s="5">
-        <v>2865600</v>
+        <v>0.14560000000000001</v>
       </c>
       <c r="J6" s="6">
         <f>I6/E6</f>
-        <v>0.12</v>
-      </c>
-      <c r="K6" s="7"/>
+        <v>5.49433962264151E-2</v>
+      </c>
+      <c r="K6" s="7">
+        <v>2.12</v>
+      </c>
       <c r="L6" s="8">
-        <v>44911</v>
+        <v>44925</v>
       </c>
       <c r="M6" s="17">
-        <v>0.62484472049689443</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
@@ -842,33 +844,33 @@
         <v>31</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="E7" s="7">
-        <v>1.75</v>
+        <v>6.49</v>
       </c>
       <c r="F7" s="6">
-        <v>0.1048451206880141</v>
+        <v>5.4538697758065524E-2</v>
       </c>
       <c r="G7" s="6">
-        <v>9.7869190335055159E-2</v>
+        <v>0.10888333370903769</v>
       </c>
       <c r="H7" s="6">
         <f>F7-G7</f>
-        <v>6.975930352958945E-3</v>
+        <v>-5.4344635950972164E-2</v>
       </c>
       <c r="I7" s="5">
-        <v>9.6099999999999991E-2</v>
+        <v>0.14560000000000001</v>
       </c>
       <c r="J7" s="6">
         <f>I7/E7</f>
-        <v>5.4914285714285707E-2</v>
+        <v>2.2434514637904468E-2</v>
       </c>
       <c r="K7" s="7">
-        <v>1.35</v>
+        <v>5.3</v>
       </c>
       <c r="L7" s="8">
-        <v>44925</v>
+        <v>45015</v>
       </c>
       <c r="M7" s="17">
         <v>3</v>
@@ -876,36 +878,36 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B8" s="5" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="E8" s="7">
-        <v>2.65</v>
+        <v>0.67</v>
       </c>
       <c r="F8" s="6">
-        <v>4.427808325428817E-2</v>
+        <v>0.1720746953370591</v>
       </c>
       <c r="G8" s="6">
-        <v>9.3811838619443283E-2</v>
+        <v>0.11018690726749793</v>
       </c>
       <c r="H8" s="6">
         <f>F8-G8</f>
-        <v>-4.9533755365155113E-2</v>
+        <v>6.1887788069561175E-2</v>
       </c>
       <c r="I8" s="5">
-        <v>0.14560000000000001</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="J8" s="6">
         <f>I8/E8</f>
-        <v>5.49433962264151E-2</v>
+        <v>0.10447761194029852</v>
       </c>
       <c r="K8" s="7">
-        <v>2.12</v>
+        <v>0.48</v>
       </c>
       <c r="L8" s="8">
         <v>44925</v>
@@ -916,42 +918,40 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B9" s="5" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="E9" s="7">
-        <v>6.49</v>
+        <v>23880000</v>
       </c>
       <c r="F9" s="6">
-        <v>5.4538697758065524E-2</v>
+        <v>6.4027111830930822E-2</v>
       </c>
       <c r="G9" s="6">
-        <v>0.10888333370903769</v>
+        <v>5.6776003015075377E-2</v>
       </c>
       <c r="H9" s="6">
         <f>F9-G9</f>
-        <v>-5.4344635950972164E-2</v>
+        <v>7.2511088158554449E-3</v>
       </c>
       <c r="I9" s="5">
-        <v>0.14560000000000001</v>
+        <v>2865600</v>
       </c>
       <c r="J9" s="6">
         <f>I9/E9</f>
-        <v>2.2434514637904468E-2</v>
-      </c>
-      <c r="K9" s="7">
-        <v>5.3</v>
-      </c>
+        <v>0.12</v>
+      </c>
+      <c r="K9" s="7"/>
       <c r="L9" s="8">
-        <v>45015</v>
+        <v>44903</v>
       </c>
       <c r="M9" s="17">
-        <v>3</v>
+        <v>0.62484472049689443</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
@@ -3643,8 +3643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA8F8C16-C341-4E22-B58A-1C8A959287DB}">
   <dimension ref="A2:J200"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3657,7 +3657,7 @@
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="13" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
@@ -3665,31 +3665,31 @@
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
       <c r="H2" s="16" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I2" s="20">
-        <v>44903</v>
+        <v>44904</v>
       </c>
       <c r="J2" s="20"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B3" s="10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D3" s="18"/>
       <c r="E3" s="19"/>
       <c r="F3" s="12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B4" s="10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D4" s="21"/>
       <c r="E4" s="22"/>
       <c r="F4" s="11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
@@ -3703,36 +3703,36 @@
         <v>3</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B7" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F7" s="7">
         <v>1.7</v>
@@ -3749,16 +3749,16 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B8" s="5" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F8" s="7">
         <v>2.2999999999999998</v>

</xml_diff>